<commit_message>
Sprint 1: bd chart
</commit_message>
<xml_diff>
--- a/planning/BurndownChart.xlsx
+++ b/planning/BurndownChart.xlsx
@@ -149,17 +149,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -369,49 +369,49 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>16</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -528,49 +528,49 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.1</c:v>
+                  <c:v>32.6666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25.1</c:v>
+                  <c:v>30.333333400000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.1</c:v>
+                  <c:v>28.000000100000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.1</c:v>
+                  <c:v>25.666666800000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.100000000000001</c:v>
+                  <c:v>23.333333500000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.100000000000001</c:v>
+                  <c:v>21.000000200000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.100000000000001</c:v>
+                  <c:v>18.666666900000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.100000000000001</c:v>
+                  <c:v>16.333333600000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.100000000000001</c:v>
+                  <c:v>14.000000300000004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.1000000000000014</c:v>
+                  <c:v>11.666667000000004</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1000000000000014</c:v>
+                  <c:v>9.3333337000000043</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.1000000000000014</c:v>
+                  <c:v>7.0000004000000047</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.1000000000000014</c:v>
+                  <c:v>4.6666671000000051</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.1000000000000014</c:v>
+                  <c:v>2.333333800000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1954,16 +1954,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>215266</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>55245</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2333,7 +2333,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2367,7 +2369,7 @@
     <col min="28" max="28" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="21" x14ac:dyDescent="0.4">
@@ -2380,150 +2382,150 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>43061</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
         <v>43062</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
         <v>43063</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
         <v>43064</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
         <v>43065</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
         <v>43066</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
         <v>43067</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
         <v>43068</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
         <v>43069</v>
       </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5">
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
         <v>43070</v>
       </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5">
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
         <v>43071</v>
       </c>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5">
+      <c r="W5" s="6"/>
+      <c r="X5" s="6">
         <v>43072</v>
       </c>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5">
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
         <v>43073</v>
       </c>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5">
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6">
         <v>43074</v>
       </c>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5">
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6">
         <v>43075</v>
       </c>
-      <c r="AE5" s="5"/>
+      <c r="AE5" s="6"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="7">
         <f>SUM(C11:C45)</f>
         <v>2</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
         <f>SUM(E11:E45)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
         <f>SUM(G11:G45)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
         <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
         <v>1</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <f>SUM(K11:K45)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
         <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
         <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4">
+      <c r="O6" s="7"/>
+      <c r="P6" s="7">
         <f>SUM(Q11:Q45)</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4">
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7">
         <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4">
+      <c r="S6" s="7"/>
+      <c r="T6" s="7">
         <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4">
+      <c r="U6" s="7"/>
+      <c r="V6" s="7">
         <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4">
+      <c r="W6" s="7"/>
+      <c r="X6" s="7">
         <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4">
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7">
         <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4">
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7">
         <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
         <v>1</v>
       </c>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4">
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7">
         <f>SUM(AE11:AE45)</f>
         <v>3</v>
       </c>
-      <c r="AE6" s="4"/>
+      <c r="AE6" s="7"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -2531,11 +2533,11 @@
       </c>
       <c r="B8">
         <f>B3-(SUM(B6:AE6))</f>
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2630,7 +2632,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="3">
         <v>12</v>
       </c>
@@ -2673,7 +2675,7 @@
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="3">
         <v>13</v>
       </c>
@@ -2700,7 +2702,7 @@
       <c r="AD12" s="3"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
@@ -2723,7 +2725,7 @@
       <c r="AD13" s="3"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -2746,7 +2748,7 @@
       <c r="AD14" s="3"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -2763,7 +2765,7 @@
       <c r="AD15" s="3"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
@@ -2781,7 +2783,7 @@
       <c r="AD16" s="3"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
@@ -2799,7 +2801,7 @@
       <c r="AD17" s="3"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
@@ -2817,7 +2819,7 @@
       <c r="AD18" s="3"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
@@ -2835,7 +2837,7 @@
       <c r="AD19" s="3"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
@@ -2853,7 +2855,7 @@
       <c r="AD20" s="3"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
@@ -2871,7 +2873,7 @@
       <c r="AD21" s="3"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
@@ -2889,7 +2891,7 @@
       <c r="AD22" s="3"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
@@ -2907,7 +2909,7 @@
       <c r="AD23" s="3"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
@@ -2925,7 +2927,7 @@
       <c r="AD24" s="3"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
@@ -2943,7 +2945,7 @@
       <c r="AD25" s="3"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
@@ -2961,7 +2963,7 @@
       <c r="AD26" s="3"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
@@ -2979,7 +2981,7 @@
       <c r="AD27" s="3"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
@@ -2997,7 +2999,7 @@
       <c r="AD28" s="3"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
@@ -3015,7 +3017,7 @@
       <c r="AD29" s="3"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
@@ -3033,7 +3035,7 @@
       <c r="AD30" s="3"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
@@ -3051,7 +3053,7 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
@@ -3069,7 +3071,7 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
@@ -3087,7 +3089,7 @@
       <c r="AD33" s="3"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
@@ -3105,7 +3107,7 @@
       <c r="AD34" s="3"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
@@ -3123,7 +3125,7 @@
       <c r="AD35" s="3"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
@@ -3141,7 +3143,7 @@
       <c r="AD36" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
@@ -3159,7 +3161,7 @@
       <c r="AD37" s="3"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
@@ -3177,7 +3179,7 @@
       <c r="AD38" s="3"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
@@ -3195,7 +3197,7 @@
       <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
@@ -3213,7 +3215,7 @@
       <c r="AD40" s="3"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
@@ -3231,7 +3233,7 @@
       <c r="AD41" s="3"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
@@ -3249,7 +3251,7 @@
       <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
@@ -3267,7 +3269,7 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
@@ -3285,7 +3287,7 @@
       <c r="AD44" s="3"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
@@ -3303,229 +3305,289 @@
       <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="5">
+      <c r="B46" s="6">
         <v>43061</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
         <v>43062</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5">
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
         <v>43063</v>
       </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
         <v>43064</v>
       </c>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5">
+      <c r="I46" s="6"/>
+      <c r="J46" s="6">
         <v>43065</v>
       </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5">
+      <c r="K46" s="6"/>
+      <c r="L46" s="6">
         <v>43066</v>
       </c>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5">
+      <c r="M46" s="6"/>
+      <c r="N46" s="6">
         <v>43067</v>
       </c>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5">
+      <c r="O46" s="6"/>
+      <c r="P46" s="6">
         <v>43068</v>
       </c>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5">
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6">
         <v>43069</v>
       </c>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5">
+      <c r="S46" s="6"/>
+      <c r="T46" s="6">
         <v>43070</v>
       </c>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5">
+      <c r="U46" s="6"/>
+      <c r="V46" s="6">
         <v>43071</v>
       </c>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5">
+      <c r="W46" s="6"/>
+      <c r="X46" s="6">
         <v>43072</v>
       </c>
-      <c r="Y46" s="5"/>
-      <c r="Z46" s="5">
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6">
         <v>43073</v>
       </c>
-      <c r="AA46" s="5"/>
-      <c r="AB46" s="5">
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6">
         <v>43074</v>
       </c>
-      <c r="AC46" s="5"/>
-      <c r="AD46" s="5">
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6">
         <v>43075</v>
       </c>
-      <c r="AE46" s="5"/>
+      <c r="AE46" s="6"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <f>$B$3-B6</f>
-        <v>27</v>
-      </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6">
+        <v>33</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
         <f>B47-D6</f>
-        <v>27</v>
-      </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6">
+        <v>33</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
         <f>D47-F6</f>
-        <v>27</v>
-      </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6">
+        <v>33</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
         <f>F47-H6</f>
-        <v>26</v>
-      </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6">
+        <v>32</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
         <f>H47-J6</f>
-        <v>26</v>
-      </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6">
+        <v>32</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5">
         <f>J47-L6</f>
-        <v>26</v>
-      </c>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6">
+        <v>32</v>
+      </c>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5">
         <f>L47-N6</f>
-        <v>26</v>
-      </c>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6">
+        <v>32</v>
+      </c>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5">
         <f>N47-P6</f>
-        <v>16</v>
-      </c>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6">
+        <v>22</v>
+      </c>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5">
         <f>P47-R6</f>
-        <v>16</v>
-      </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6">
+        <v>22</v>
+      </c>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5">
         <f>R47-T6</f>
-        <v>16</v>
-      </c>
-      <c r="U47" s="6"/>
-      <c r="V47" s="6">
+        <v>22</v>
+      </c>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5">
         <f>T47-V6</f>
-        <v>16</v>
-      </c>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6">
+        <v>22</v>
+      </c>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5">
         <f>V47-X6</f>
-        <v>16</v>
-      </c>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6">
+        <v>22</v>
+      </c>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5">
         <f>X47-Z6</f>
-        <v>16</v>
-      </c>
-      <c r="AA47" s="6"/>
-      <c r="AB47" s="6">
+        <v>22</v>
+      </c>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5">
         <f>Z47-AB6</f>
-        <v>15</v>
-      </c>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6">
+        <v>21</v>
+      </c>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5">
         <f>AB47-AD6</f>
-        <v>12</v>
-      </c>
-      <c r="AE47" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="AE47" s="5"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <f>B3</f>
-        <v>29</v>
-      </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6">
-        <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),1))</f>
-        <v>27.1</v>
-      </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6">
-        <f>D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>25.1</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6">
-        <f>F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>23.1</v>
-      </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6">
-        <f>H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>21.1</v>
-      </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6">
-        <f>J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>19.100000000000001</v>
-      </c>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6">
-        <f>L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>17.100000000000001</v>
-      </c>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6">
-        <f>N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>15.100000000000001</v>
-      </c>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6">
-        <f>P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>13.100000000000001</v>
-      </c>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6">
-        <f>R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>11.100000000000001</v>
-      </c>
-      <c r="U48" s="6"/>
-      <c r="V48" s="6">
-        <f>T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>9.1000000000000014</v>
-      </c>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6">
-        <f>V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>7.1000000000000014</v>
-      </c>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6">
-        <f>X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>5.1000000000000014</v>
-      </c>
-      <c r="AA48" s="6"/>
-      <c r="AB48" s="6">
-        <f>Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>3.1000000000000014</v>
-      </c>
-      <c r="AC48" s="6"/>
-      <c r="AD48" s="6">
-        <f>AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),0))</f>
-        <v>1.1000000000000014</v>
-      </c>
-      <c r="AE48" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
+        <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>32.6666667</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5">
+        <f t="shared" ref="F48" si="9">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>30.333333400000001</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5">
+        <f t="shared" ref="H48" si="10">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>28.000000100000001</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
+        <f t="shared" ref="J48" si="11">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>25.666666800000002</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5">
+        <f t="shared" ref="L48" si="12">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>23.333333500000002</v>
+      </c>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5">
+        <f t="shared" ref="N48" si="13">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>21.000000200000002</v>
+      </c>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5">
+        <f t="shared" ref="P48" si="14">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>18.666666900000003</v>
+      </c>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5">
+        <f t="shared" ref="R48" si="15">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>16.333333600000003</v>
+      </c>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5">
+        <f t="shared" ref="T48" si="16">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>14.000000300000004</v>
+      </c>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5">
+        <f t="shared" ref="V48" si="17">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>11.666667000000004</v>
+      </c>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5">
+        <f t="shared" ref="X48" si="18">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>9.3333337000000043</v>
+      </c>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5">
+        <f t="shared" ref="Z48" si="19">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>7.0000004000000047</v>
+      </c>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5">
+        <f t="shared" ref="AB48" si="20">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>4.6666671000000051</v>
+      </c>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5">
+        <f t="shared" ref="AD48" si="21">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),7))</f>
+        <v>2.333333800000005</v>
+      </c>
+      <c r="AE48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="A10:A45"/>
     <mergeCell ref="T48:U48"/>
     <mergeCell ref="T47:U47"/>
@@ -3542,66 +3604,6 @@
     <mergeCell ref="AD48:AE48"/>
     <mergeCell ref="AB48:AC48"/>
     <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB46:AC46"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
@@ -3666,146 +3668,146 @@
       </c>
     </row>
     <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+      <c r="B5" s="6">
         <v>43061</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
         <v>43062</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
         <v>43063</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
         <v>43064</v>
       </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
         <v>43065</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
         <v>43066</v>
       </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
         <v>43067</v>
       </c>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
         <v>43068</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
         <v>43069</v>
       </c>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5">
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
         <v>43070</v>
       </c>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5">
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
         <v>43071</v>
       </c>
-      <c r="W5" s="5"/>
-      <c r="X5" s="5">
+      <c r="W5" s="6"/>
+      <c r="X5" s="6">
         <v>43072</v>
       </c>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="5">
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
         <v>43073</v>
       </c>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="5">
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6">
         <v>43074</v>
       </c>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="5">
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6">
         <v>43075</v>
       </c>
-      <c r="AE5" s="5"/>
+      <c r="AE5" s="6"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="7">
         <f>SUM(C11:C45)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
         <f>SUM(E11:E45)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
         <f>SUM(G11:G45)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
         <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <f>SUM(K11:K45)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
         <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
         <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4">
+      <c r="O6" s="7"/>
+      <c r="P6" s="7">
         <f>SUM(Q11:Q45)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4">
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7">
         <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4">
+      <c r="S6" s="7"/>
+      <c r="T6" s="7">
         <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4">
+      <c r="U6" s="7"/>
+      <c r="V6" s="7">
         <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4">
+      <c r="W6" s="7"/>
+      <c r="X6" s="7">
         <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4">
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7">
         <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="4">
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7">
         <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4">
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7">
         <f t="shared" ref="AD6" si="9">SUM(AE11:AE45)</f>
         <v>0</v>
       </c>
-      <c r="AE6" s="4"/>
+      <c r="AE6" s="7"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -3817,7 +3819,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3912,7 +3914,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="3"/>
@@ -3930,7 +3932,7 @@
       <c r="AD11" s="3"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="3"/>
@@ -3948,7 +3950,7 @@
       <c r="AD12" s="3"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
@@ -3966,7 +3968,7 @@
       <c r="AD13" s="3"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -3984,7 +3986,7 @@
       <c r="AD14" s="3"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -4001,7 +4003,7 @@
       <c r="AD15" s="3"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
@@ -4019,7 +4021,7 @@
       <c r="AD16" s="3"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
@@ -4037,7 +4039,7 @@
       <c r="AD17" s="3"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
@@ -4055,7 +4057,7 @@
       <c r="AD18" s="3"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
@@ -4073,7 +4075,7 @@
       <c r="AD19" s="3"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
@@ -4091,7 +4093,7 @@
       <c r="AD20" s="3"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
@@ -4109,7 +4111,7 @@
       <c r="AD21" s="3"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
@@ -4127,7 +4129,7 @@
       <c r="AD22" s="3"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
@@ -4145,7 +4147,7 @@
       <c r="AD23" s="3"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
@@ -4163,7 +4165,7 @@
       <c r="AD24" s="3"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
@@ -4181,7 +4183,7 @@
       <c r="AD25" s="3"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
@@ -4199,7 +4201,7 @@
       <c r="AD26" s="3"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
@@ -4217,7 +4219,7 @@
       <c r="AD27" s="3"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
@@ -4235,7 +4237,7 @@
       <c r="AD28" s="3"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
@@ -4253,7 +4255,7 @@
       <c r="AD29" s="3"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
@@ -4271,7 +4273,7 @@
       <c r="AD30" s="3"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
@@ -4289,7 +4291,7 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
@@ -4307,7 +4309,7 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
@@ -4325,7 +4327,7 @@
       <c r="AD33" s="3"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
@@ -4343,7 +4345,7 @@
       <c r="AD34" s="3"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
@@ -4361,7 +4363,7 @@
       <c r="AD35" s="3"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
@@ -4379,7 +4381,7 @@
       <c r="AD36" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
@@ -4397,7 +4399,7 @@
       <c r="AD37" s="3"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
@@ -4415,7 +4417,7 @@
       <c r="AD38" s="3"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
@@ -4433,7 +4435,7 @@
       <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
@@ -4451,7 +4453,7 @@
       <c r="AD40" s="3"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
@@ -4469,7 +4471,7 @@
       <c r="AD41" s="3"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
@@ -4487,7 +4489,7 @@
       <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
@@ -4505,7 +4507,7 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
@@ -4523,7 +4525,7 @@
       <c r="AD44" s="3"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
@@ -4541,234 +4543,284 @@
       <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="5">
+      <c r="B46" s="6">
         <v>43061</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
         <v>43062</v>
       </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5">
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
         <v>43063</v>
       </c>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
         <v>43064</v>
       </c>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5">
+      <c r="I46" s="6"/>
+      <c r="J46" s="6">
         <v>43065</v>
       </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5">
+      <c r="K46" s="6"/>
+      <c r="L46" s="6">
         <v>43066</v>
       </c>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5">
+      <c r="M46" s="6"/>
+      <c r="N46" s="6">
         <v>43067</v>
       </c>
-      <c r="O46" s="5"/>
-      <c r="P46" s="5">
+      <c r="O46" s="6"/>
+      <c r="P46" s="6">
         <v>43068</v>
       </c>
-      <c r="Q46" s="5"/>
-      <c r="R46" s="5">
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6">
         <v>43069</v>
       </c>
-      <c r="S46" s="5"/>
-      <c r="T46" s="5">
+      <c r="S46" s="6"/>
+      <c r="T46" s="6">
         <v>43070</v>
       </c>
-      <c r="U46" s="5"/>
-      <c r="V46" s="5">
+      <c r="U46" s="6"/>
+      <c r="V46" s="6">
         <v>43071</v>
       </c>
-      <c r="W46" s="5"/>
-      <c r="X46" s="5">
+      <c r="W46" s="6"/>
+      <c r="X46" s="6">
         <v>43072</v>
       </c>
-      <c r="Y46" s="5"/>
-      <c r="Z46" s="5">
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6">
         <v>43073</v>
       </c>
-      <c r="AA46" s="5"/>
-      <c r="AB46" s="5">
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6">
         <v>43074</v>
       </c>
-      <c r="AC46" s="5"/>
-      <c r="AD46" s="5">
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6">
         <v>43075</v>
       </c>
-      <c r="AE46" s="5"/>
+      <c r="AE46" s="6"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <f>$B$3-B6</f>
         <v>25</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
         <f>B47-D6</f>
         <v>25</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
         <f>D47-F6</f>
         <v>25</v>
       </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6">
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
         <f>F47-H6</f>
         <v>25</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6">
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
         <f>H47-J6</f>
         <v>25</v>
       </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6">
+      <c r="K47" s="5"/>
+      <c r="L47" s="5">
         <f>J47-L6</f>
         <v>25</v>
       </c>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6">
+      <c r="M47" s="5"/>
+      <c r="N47" s="5">
         <f>L47-N6</f>
         <v>25</v>
       </c>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6">
+      <c r="O47" s="5"/>
+      <c r="P47" s="5">
         <f>N47-P6</f>
         <v>25</v>
       </c>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6">
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5">
         <f>P47-R6</f>
         <v>25</v>
       </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6">
+      <c r="S47" s="5"/>
+      <c r="T47" s="5">
         <f>R47-T6</f>
         <v>25</v>
       </c>
-      <c r="U47" s="6"/>
-      <c r="V47" s="6">
+      <c r="U47" s="5"/>
+      <c r="V47" s="5">
         <f>T47-V6</f>
         <v>25</v>
       </c>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6">
+      <c r="W47" s="5"/>
+      <c r="X47" s="5">
         <f>V47-X6</f>
         <v>25</v>
       </c>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6">
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5">
         <f>X47-Z6</f>
         <v>25</v>
       </c>
-      <c r="AA47" s="6"/>
-      <c r="AB47" s="6">
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5">
         <f>Z47-AB6</f>
         <v>25</v>
       </c>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6">
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5">
         <f>AB47-AD6</f>
         <v>25</v>
       </c>
-      <c r="AE47" s="6"/>
+      <c r="AE47" s="5"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <f>B3</f>
         <v>25</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
         <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>23.33</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5">
         <f t="shared" ref="F48" si="10">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>21.659999999999997</v>
       </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6">
+      <c r="G48" s="5"/>
+      <c r="H48" s="5">
         <f t="shared" ref="H48" si="11">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>19.989999999999995</v>
       </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6">
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
         <f t="shared" ref="J48" si="12">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>18.319999999999993</v>
       </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6">
+      <c r="K48" s="5"/>
+      <c r="L48" s="5">
         <f t="shared" ref="L48" si="13">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>16.649999999999991</v>
       </c>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6">
+      <c r="M48" s="5"/>
+      <c r="N48" s="5">
         <f t="shared" ref="N48" si="14">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>14.979999999999992</v>
       </c>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6">
+      <c r="O48" s="5"/>
+      <c r="P48" s="5">
         <f t="shared" ref="P48" si="15">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>13.309999999999992</v>
       </c>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6">
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5">
         <f t="shared" ref="R48" si="16">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>11.639999999999992</v>
       </c>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6">
+      <c r="S48" s="5"/>
+      <c r="T48" s="5">
         <f t="shared" ref="T48" si="17">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>9.9699999999999918</v>
       </c>
-      <c r="U48" s="6"/>
-      <c r="V48" s="6">
+      <c r="U48" s="5"/>
+      <c r="V48" s="5">
         <f t="shared" ref="V48" si="18">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>8.2999999999999918</v>
       </c>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6">
+      <c r="W48" s="5"/>
+      <c r="X48" s="5">
         <f t="shared" ref="X48" si="19">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>6.6299999999999919</v>
       </c>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6">
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5">
         <f t="shared" ref="Z48" si="20">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>4.959999999999992</v>
       </c>
-      <c r="AA48" s="6"/>
-      <c r="AB48" s="6">
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5">
         <f t="shared" ref="AB48" si="21">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>3.289999999999992</v>
       </c>
-      <c r="AC48" s="6"/>
-      <c r="AD48" s="6">
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5">
         <f t="shared" ref="AD48" si="22">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>1.6199999999999921</v>
       </c>
-      <c r="AE48" s="6"/>
+      <c r="AE48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="T48:U48"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="X48:Y48"/>
-    <mergeCell ref="Z48:AA48"/>
-    <mergeCell ref="AB48:AC48"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Z46:AA46"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="A10:A45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="AD46:AE46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="T46:U46"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="X46:Y46"/>
     <mergeCell ref="AD48:AE48"/>
     <mergeCell ref="AD47:AE47"/>
     <mergeCell ref="B48:C48"/>
@@ -4785,61 +4837,11 @@
     <mergeCell ref="V47:W47"/>
     <mergeCell ref="X47:Y47"/>
     <mergeCell ref="Z47:AA47"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AB46:AC46"/>
-    <mergeCell ref="AD46:AE46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="T46:U46"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="X46:Y46"/>
-    <mergeCell ref="Z46:AA46"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="A10:A45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="X48:Y48"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="AB48:AC48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Sprint 2: bd chart
</commit_message>
<xml_diff>
--- a/planning/BurndownChart.xlsx
+++ b/planning/BurndownChart.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
-    <sheet name="Sprint Burndown Chart Template" sheetId="3" r:id="rId2"/>
+    <sheet name="Sprint 2 Burndown Chart" sheetId="4" r:id="rId2"/>
+    <sheet name="Sprint Burndown Chart Template" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="10">
   <si>
     <t>effort remaining</t>
   </si>
@@ -75,6 +76,9 @@
 -Beim Ticket nur die Nr hinschreiben, Hashtag wird generiert.
 -Amout = unser Rating (gelbes Label)</t>
     </r>
+  </si>
+  <si>
+    <t>Sprint 2 Burndown Chart</t>
   </si>
 </sst>
 </file>
@@ -149,17 +153,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,7 +415,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -834,6 +838,614 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH" baseline="0"/>
+              <a:t> Chart Sprint 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2 Burndown Chart'!$A$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>effort remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2 Burndown Chart'!$B$46:$AE$46</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>43075</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43077</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43078</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43079</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43080</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43081</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43082</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43083</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43084</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43085</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43086</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43087</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43088</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2 Burndown Chart'!$B$47:$AE$47</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4CD-466F-983C-BBC1244ADCE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 2 Burndown Chart'!$A$48</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ideal effort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:tint val="77000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 2 Burndown Chart'!$B$46:$AE$46</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>43075</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43077</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43078</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43079</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43080</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43081</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>43082</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>43083</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43084</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43085</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>43086</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>43087</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>43088</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43089</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 2 Burndown Chart'!$B$48:$AE$48</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.659999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.989999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.319999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.649999999999991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.979999999999992</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.309999999999992</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.639999999999992</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.9699999999999918</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.2999999999999918</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.6299999999999919</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.959999999999992</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.289999999999992</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6199999999999921</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F4CD-466F-983C-BBC1244ADCE3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="48858624"/>
+        <c:axId val="48860544"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="48858624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="48860544"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="48860544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-CH"/>
+                  <a:t>Effort</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="48858624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -1955,15 +2567,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>314326</xdr:colOff>
+      <xdr:colOff>139066</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>102870</xdr:rowOff>
+      <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>55245</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1992,6 +2604,49 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>474346</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>169545</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC2969C4-0459-4CC3-8DF2-401BCBA151AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2333,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2386,146 +3041,146 @@
       </c>
     </row>
     <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>43061</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
         <v>43062</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
         <v>43063</v>
       </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
         <v>43064</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4">
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
         <v>43065</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4">
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
         <v>43066</v>
       </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4">
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
         <v>43067</v>
       </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4">
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
         <v>43068</v>
       </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
         <v>43069</v>
       </c>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4">
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
         <v>43070</v>
       </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4">
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
         <v>43071</v>
       </c>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4">
+      <c r="W5" s="6"/>
+      <c r="X5" s="6">
         <v>43072</v>
       </c>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4">
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
         <v>43073</v>
       </c>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4">
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6">
         <v>43074</v>
       </c>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4">
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6">
         <v>43075</v>
       </c>
-      <c r="AE5" s="4"/>
+      <c r="AE5" s="6"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <f>SUM(C11:C45)</f>
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
         <f>SUM(E11:E45)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
         <f>SUM(G11:G45)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
         <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
         <v>1</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <f>SUM(K11:K45)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
         <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
         <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5">
+      <c r="O6" s="7"/>
+      <c r="P6" s="7">
         <f>SUM(Q11:Q45)</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5">
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7">
         <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5">
+      <c r="S6" s="7"/>
+      <c r="T6" s="7">
         <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5">
+      <c r="U6" s="7"/>
+      <c r="V6" s="7">
         <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5">
+      <c r="W6" s="7"/>
+      <c r="X6" s="7">
         <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5">
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7">
         <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5">
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7">
         <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
         <v>1</v>
       </c>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5">
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7">
         <f>SUM(AE11:AE45)</f>
-        <v>11</v>
-      </c>
-      <c r="AE6" s="5"/>
+        <v>21</v>
+      </c>
+      <c r="AE6" s="7"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -2533,11 +3188,11 @@
       </c>
       <c r="B8">
         <f>B3-(SUM(B6:AE6))</f>
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2632,7 +3287,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="3">
         <v>12</v>
       </c>
@@ -2675,7 +3330,7 @@
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="3">
         <v>13</v>
       </c>
@@ -2707,7 +3362,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
@@ -2735,7 +3390,7 @@
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -2755,10 +3410,15 @@
       <c r="X14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AB14" s="3"/>
-      <c r="AD14" s="3"/>
+      <c r="AD14" s="3">
+        <v>9</v>
+      </c>
+      <c r="AE14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -2772,10 +3432,15 @@
       <c r="X15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AB15" s="3"/>
-      <c r="AD15" s="3"/>
+      <c r="AD15" s="3">
+        <v>7</v>
+      </c>
+      <c r="AE15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
@@ -2790,10 +3455,15 @@
       <c r="X16" s="3"/>
       <c r="Z16" s="3"/>
       <c r="AB16" s="3"/>
-      <c r="AD16" s="3"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="AD16" s="3">
+        <v>41</v>
+      </c>
+      <c r="AE16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
@@ -2808,10 +3478,15 @@
       <c r="X17" s="3"/>
       <c r="Z17" s="3"/>
       <c r="AB17" s="3"/>
-      <c r="AD17" s="3"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="AD17" s="3">
+        <v>42</v>
+      </c>
+      <c r="AE17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
@@ -2828,8 +3503,8 @@
       <c r="AB18" s="3"/>
       <c r="AD18" s="3"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="3"/>
@@ -2845,8 +3520,8 @@
       <c r="AB19" s="3"/>
       <c r="AD19" s="3"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
       <c r="H20" s="3"/>
@@ -2862,8 +3537,8 @@
       <c r="AB20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
@@ -2880,8 +3555,8 @@
       <c r="AB21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
@@ -2898,8 +3573,8 @@
       <c r="AB22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
@@ -2916,8 +3591,8 @@
       <c r="AB23" s="3"/>
       <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
@@ -2934,8 +3609,8 @@
       <c r="AB24" s="3"/>
       <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
@@ -2952,8 +3627,8 @@
       <c r="AB25" s="3"/>
       <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
@@ -2970,8 +3645,8 @@
       <c r="AB26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
@@ -2988,8 +3663,8 @@
       <c r="AB27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
@@ -3006,8 +3681,8 @@
       <c r="AB28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
@@ -3024,8 +3699,8 @@
       <c r="AB29" s="3"/>
       <c r="AD29" s="3"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
@@ -3042,8 +3717,8 @@
       <c r="AB30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
@@ -3060,8 +3735,8 @@
       <c r="AB31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
@@ -3079,7 +3754,7 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
@@ -3097,7 +3772,7 @@
       <c r="AD33" s="3"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
@@ -3115,7 +3790,7 @@
       <c r="AD34" s="3"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
@@ -3133,7 +3808,7 @@
       <c r="AD35" s="3"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
@@ -3151,7 +3826,7 @@
       <c r="AD36" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
@@ -3169,7 +3844,7 @@
       <c r="AD37" s="3"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
@@ -3187,7 +3862,7 @@
       <c r="AD38" s="3"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
@@ -3205,7 +3880,7 @@
       <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
@@ -3223,7 +3898,7 @@
       <c r="AD40" s="3"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
@@ -3241,7 +3916,7 @@
       <c r="AD41" s="3"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
@@ -3259,7 +3934,7 @@
       <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
@@ -3277,7 +3952,7 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
@@ -3295,7 +3970,7 @@
       <c r="AD44" s="3"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
@@ -3313,215 +3988,275 @@
       <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="4">
+      <c r="B46" s="6">
         <v>43061</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
         <v>43062</v>
       </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4">
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
         <v>43063</v>
       </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
         <v>43064</v>
       </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4">
+      <c r="I46" s="6"/>
+      <c r="J46" s="6">
         <v>43065</v>
       </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4">
+      <c r="K46" s="6"/>
+      <c r="L46" s="6">
         <v>43066</v>
       </c>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4">
+      <c r="M46" s="6"/>
+      <c r="N46" s="6">
         <v>43067</v>
       </c>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4">
+      <c r="O46" s="6"/>
+      <c r="P46" s="6">
         <v>43068</v>
       </c>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4">
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6">
         <v>43069</v>
       </c>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4">
+      <c r="S46" s="6"/>
+      <c r="T46" s="6">
         <v>43070</v>
       </c>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4">
+      <c r="U46" s="6"/>
+      <c r="V46" s="6">
         <v>43071</v>
       </c>
-      <c r="W46" s="4"/>
-      <c r="X46" s="4">
+      <c r="W46" s="6"/>
+      <c r="X46" s="6">
         <v>43072</v>
       </c>
-      <c r="Y46" s="4"/>
-      <c r="Z46" s="4">
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6">
         <v>43073</v>
       </c>
-      <c r="AA46" s="4"/>
-      <c r="AB46" s="4">
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6">
         <v>43074</v>
       </c>
-      <c r="AC46" s="4"/>
-      <c r="AD46" s="4">
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6">
         <v>43075</v>
       </c>
-      <c r="AE46" s="4"/>
+      <c r="AE46" s="6"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <f>$B$3-B6</f>
         <v>33</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
         <f>B47-D6</f>
         <v>33</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
         <f>D47-F6</f>
         <v>33</v>
       </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6">
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
         <f>F47-H6</f>
         <v>32</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6">
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
         <f>H47-J6</f>
         <v>32</v>
       </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6">
+      <c r="K47" s="5"/>
+      <c r="L47" s="5">
         <f>J47-L6</f>
         <v>32</v>
       </c>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6">
+      <c r="M47" s="5"/>
+      <c r="N47" s="5">
         <f>L47-N6</f>
         <v>32</v>
       </c>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6">
+      <c r="O47" s="5"/>
+      <c r="P47" s="5">
         <f>N47-P6</f>
         <v>22</v>
       </c>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6">
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5">
         <f>P47-R6</f>
         <v>22</v>
       </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6">
+      <c r="S47" s="5"/>
+      <c r="T47" s="5">
         <f>R47-T6</f>
         <v>22</v>
       </c>
-      <c r="U47" s="6"/>
-      <c r="V47" s="6">
+      <c r="U47" s="5"/>
+      <c r="V47" s="5">
         <f>T47-V6</f>
         <v>22</v>
       </c>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6">
+      <c r="W47" s="5"/>
+      <c r="X47" s="5">
         <f>V47-X6</f>
         <v>22</v>
       </c>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6">
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5">
         <f>X47-Z6</f>
         <v>22</v>
       </c>
-      <c r="AA47" s="6"/>
-      <c r="AB47" s="6">
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5">
         <f>Z47-AB6</f>
         <v>21</v>
       </c>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6">
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5">
         <f>AB47-AD6</f>
-        <v>10</v>
-      </c>
-      <c r="AE47" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE47" s="5"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <f>B3</f>
         <v>35</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
         <v>32.5</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5">
         <v>30</v>
       </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6">
+      <c r="G48" s="5"/>
+      <c r="H48" s="5">
         <v>27.5</v>
       </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6">
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
         <v>25</v>
       </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6">
+      <c r="K48" s="5"/>
+      <c r="L48" s="5">
         <v>22</v>
       </c>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6">
+      <c r="M48" s="5"/>
+      <c r="N48" s="5">
         <v>19.5</v>
       </c>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6">
+      <c r="O48" s="5"/>
+      <c r="P48" s="5">
         <v>17</v>
       </c>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6">
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5">
         <v>14.5</v>
       </c>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6">
+      <c r="S48" s="5"/>
+      <c r="T48" s="5">
         <v>12</v>
       </c>
-      <c r="U48" s="6"/>
-      <c r="V48" s="6">
+      <c r="U48" s="5"/>
+      <c r="V48" s="5">
         <v>9.5</v>
       </c>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6">
+      <c r="W48" s="5"/>
+      <c r="X48" s="5">
         <v>7</v>
       </c>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6">
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5">
         <v>4.5</v>
       </c>
-      <c r="AA48" s="6"/>
-      <c r="AB48" s="6">
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5">
         <v>2</v>
       </c>
-      <c r="AC48" s="6"/>
-      <c r="AD48" s="6">
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5">
         <v>0</v>
       </c>
-      <c r="AE48" s="6"/>
+      <c r="AE48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z5:AA5"/>
     <mergeCell ref="A10:A45"/>
     <mergeCell ref="T48:U48"/>
     <mergeCell ref="T47:U47"/>
@@ -3538,66 +4273,6 @@
     <mergeCell ref="AD48:AE48"/>
     <mergeCell ref="AB48:AC48"/>
     <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB46:AC46"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
@@ -3606,11 +4281,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE7739D-713E-4D3F-8C3C-20CB148605F1}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L41" sqref="L41"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3650,7 +4325,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -3662,146 +4337,146 @@
       </c>
     </row>
     <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="4">
-        <v>43061</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4">
-        <v>43062</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4">
-        <v>43063</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4">
-        <v>43064</v>
-      </c>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4">
-        <v>43065</v>
-      </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4">
-        <v>43066</v>
-      </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4">
-        <v>43067</v>
-      </c>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4">
-        <v>43068</v>
-      </c>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4">
-        <v>43069</v>
-      </c>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4">
-        <v>43070</v>
-      </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4">
-        <v>43071</v>
-      </c>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4">
-        <v>43072</v>
-      </c>
-      <c r="Y5" s="4"/>
-      <c r="Z5" s="4">
-        <v>43073</v>
-      </c>
-      <c r="AA5" s="4"/>
-      <c r="AB5" s="4">
-        <v>43074</v>
-      </c>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4">
+      <c r="B5" s="6">
         <v>43075</v>
       </c>
-      <c r="AE5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
+        <v>43076</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>43077</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
+        <v>43078</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
+        <v>43079</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
+        <v>43080</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
+        <v>43081</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
+        <v>43082</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <v>43083</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
+        <v>43084</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
+        <v>43085</v>
+      </c>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6">
+        <v>43086</v>
+      </c>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
+        <v>43087</v>
+      </c>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6">
+        <v>43088</v>
+      </c>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6">
+        <v>43089</v>
+      </c>
+      <c r="AE5" s="6"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="7">
         <f>SUM(C11:C45)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
         <f>SUM(E11:E45)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
         <f>SUM(G11:G45)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5">
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
         <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5">
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
         <f>SUM(K11:K45)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5">
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
         <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5">
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
         <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5">
+      <c r="O6" s="7"/>
+      <c r="P6" s="7">
         <f>SUM(Q11:Q45)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5">
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7">
         <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5">
+      <c r="S6" s="7"/>
+      <c r="T6" s="7">
         <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5">
+      <c r="U6" s="7"/>
+      <c r="V6" s="7">
         <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="5"/>
-      <c r="X6" s="5">
+      <c r="W6" s="7"/>
+      <c r="X6" s="7">
         <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="5">
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7">
         <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="5">
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7">
         <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="5">
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7">
         <f t="shared" ref="AD6" si="9">SUM(AE11:AE45)</f>
         <v>0</v>
       </c>
-      <c r="AE6" s="5"/>
+      <c r="AE6" s="7"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -3813,7 +4488,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3908,7 +4583,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="3"/>
@@ -3926,7 +4601,7 @@
       <c r="AD11" s="3"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="3"/>
@@ -3944,7 +4619,7 @@
       <c r="AD12" s="3"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
@@ -3962,7 +4637,7 @@
       <c r="AD13" s="3"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -3980,7 +4655,7 @@
       <c r="AD14" s="3"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -3997,7 +4672,7 @@
       <c r="AD15" s="3"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
@@ -4015,7 +4690,7 @@
       <c r="AD16" s="3"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
@@ -4033,7 +4708,7 @@
       <c r="AD17" s="3"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
@@ -4051,7 +4726,7 @@
       <c r="AD18" s="3"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
@@ -4069,7 +4744,7 @@
       <c r="AD19" s="3"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
@@ -4087,7 +4762,7 @@
       <c r="AD20" s="3"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
@@ -4105,7 +4780,7 @@
       <c r="AD21" s="3"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
@@ -4123,7 +4798,7 @@
       <c r="AD22" s="3"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
+      <c r="A23" s="4"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
@@ -4141,7 +4816,7 @@
       <c r="AD23" s="3"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
@@ -4159,7 +4834,7 @@
       <c r="AD24" s="3"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
@@ -4177,7 +4852,7 @@
       <c r="AD25" s="3"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="4"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
@@ -4195,7 +4870,7 @@
       <c r="AD26" s="3"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
@@ -4213,7 +4888,7 @@
       <c r="AD27" s="3"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
@@ -4231,7 +4906,7 @@
       <c r="AD28" s="3"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
@@ -4249,7 +4924,7 @@
       <c r="AD29" s="3"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
+      <c r="A30" s="4"/>
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
@@ -4267,7 +4942,7 @@
       <c r="AD30" s="3"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
@@ -4285,7 +4960,7 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
@@ -4303,7 +4978,7 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
@@ -4321,7 +4996,7 @@
       <c r="AD33" s="3"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
@@ -4339,7 +5014,7 @@
       <c r="AD34" s="3"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
@@ -4357,7 +5032,7 @@
       <c r="AD35" s="3"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
@@ -4375,7 +5050,7 @@
       <c r="AD36" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
@@ -4393,7 +5068,7 @@
       <c r="AD37" s="3"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="4"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
@@ -4411,7 +5086,7 @@
       <c r="AD38" s="3"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
@@ -4429,7 +5104,7 @@
       <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="4"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
@@ -4447,7 +5122,7 @@
       <c r="AD40" s="3"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
@@ -4465,7 +5140,7 @@
       <c r="AD41" s="3"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
@@ -4483,7 +5158,7 @@
       <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
@@ -4501,7 +5176,7 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="4"/>
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
@@ -4519,7 +5194,7 @@
       <c r="AD44" s="3"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
@@ -4537,226 +5212,241 @@
       <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="4">
-        <v>43061</v>
-      </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4">
-        <v>43062</v>
-      </c>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4">
-        <v>43063</v>
-      </c>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4">
-        <v>43064</v>
-      </c>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4">
-        <v>43065</v>
-      </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4">
-        <v>43066</v>
-      </c>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4">
-        <v>43067</v>
-      </c>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4">
-        <v>43068</v>
-      </c>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4">
-        <v>43069</v>
-      </c>
-      <c r="S46" s="4"/>
-      <c r="T46" s="4">
-        <v>43070</v>
-      </c>
-      <c r="U46" s="4"/>
-      <c r="V46" s="4">
-        <v>43071</v>
-      </c>
-      <c r="W46" s="4"/>
-      <c r="X46" s="4">
-        <v>43072</v>
-      </c>
-      <c r="Y46" s="4"/>
-      <c r="Z46" s="4">
-        <v>43073</v>
-      </c>
-      <c r="AA46" s="4"/>
-      <c r="AB46" s="4">
-        <v>43074</v>
-      </c>
-      <c r="AC46" s="4"/>
-      <c r="AD46" s="4">
+      <c r="B46" s="6">
+        <f>B5</f>
         <v>43075</v>
       </c>
-      <c r="AE46" s="4"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
+        <f t="shared" ref="D46:AE46" si="10">D5</f>
+        <v>43076</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
+        <f t="shared" ref="F46:AE46" si="11">F5</f>
+        <v>43077</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
+        <f t="shared" ref="H46:AE46" si="12">H5</f>
+        <v>43078</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6">
+        <f t="shared" ref="J46:AE46" si="13">J5</f>
+        <v>43079</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6">
+        <f t="shared" ref="L46:AE46" si="14">L5</f>
+        <v>43080</v>
+      </c>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6">
+        <f t="shared" ref="N46:AE46" si="15">N5</f>
+        <v>43081</v>
+      </c>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6">
+        <f t="shared" ref="P46:AE46" si="16">P5</f>
+        <v>43082</v>
+      </c>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6">
+        <f t="shared" ref="R46:AE46" si="17">R5</f>
+        <v>43083</v>
+      </c>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6">
+        <f t="shared" ref="T46:AE46" si="18">T5</f>
+        <v>43084</v>
+      </c>
+      <c r="U46" s="6"/>
+      <c r="V46" s="6">
+        <f t="shared" ref="V46:AE46" si="19">V5</f>
+        <v>43085</v>
+      </c>
+      <c r="W46" s="6"/>
+      <c r="X46" s="6">
+        <f t="shared" ref="X46:AE46" si="20">X5</f>
+        <v>43086</v>
+      </c>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6">
+        <f t="shared" ref="Z46:AE46" si="21">Z5</f>
+        <v>43087</v>
+      </c>
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6">
+        <f t="shared" ref="AB46:AE46" si="22">AB5</f>
+        <v>43088</v>
+      </c>
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6">
+        <f>AD5</f>
+        <v>43089</v>
+      </c>
+      <c r="AE46" s="6"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="6">
+      <c r="B47" s="5">
         <f>$B$3-B6</f>
         <v>25</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
         <f>B47-D6</f>
         <v>25</v>
       </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6">
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
         <f>D47-F6</f>
         <v>25</v>
       </c>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6">
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
         <f>F47-H6</f>
         <v>25</v>
       </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6">
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
         <f>H47-J6</f>
         <v>25</v>
       </c>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6">
+      <c r="K47" s="5"/>
+      <c r="L47" s="5">
         <f>J47-L6</f>
         <v>25</v>
       </c>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6">
+      <c r="M47" s="5"/>
+      <c r="N47" s="5">
         <f>L47-N6</f>
         <v>25</v>
       </c>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6">
+      <c r="O47" s="5"/>
+      <c r="P47" s="5">
         <f>N47-P6</f>
         <v>25</v>
       </c>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6">
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5">
         <f>P47-R6</f>
         <v>25</v>
       </c>
-      <c r="S47" s="6"/>
-      <c r="T47" s="6">
+      <c r="S47" s="5"/>
+      <c r="T47" s="5">
         <f>R47-T6</f>
         <v>25</v>
       </c>
-      <c r="U47" s="6"/>
-      <c r="V47" s="6">
+      <c r="U47" s="5"/>
+      <c r="V47" s="5">
         <f>T47-V6</f>
         <v>25</v>
       </c>
-      <c r="W47" s="6"/>
-      <c r="X47" s="6">
+      <c r="W47" s="5"/>
+      <c r="X47" s="5">
         <f>V47-X6</f>
         <v>25</v>
       </c>
-      <c r="Y47" s="6"/>
-      <c r="Z47" s="6">
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5">
         <f>X47-Z6</f>
         <v>25</v>
       </c>
-      <c r="AA47" s="6"/>
-      <c r="AB47" s="6">
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5">
         <f>Z47-AB6</f>
         <v>25</v>
       </c>
-      <c r="AC47" s="6"/>
-      <c r="AD47" s="6">
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5">
         <f>AB47-AD6</f>
         <v>25</v>
       </c>
-      <c r="AE47" s="6"/>
+      <c r="AE47" s="5"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="6">
+      <c r="B48" s="5">
         <f>B3</f>
         <v>25</v>
       </c>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
         <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>23.33</v>
       </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6">
-        <f t="shared" ref="F48" si="10">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5">
+        <f t="shared" ref="F48" si="23">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>21.659999999999997</v>
       </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6">
-        <f t="shared" ref="H48" si="11">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5">
+        <f t="shared" ref="H48" si="24">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>19.989999999999995</v>
       </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6">
-        <f t="shared" ref="J48" si="12">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
+        <f t="shared" ref="J48" si="25">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>18.319999999999993</v>
       </c>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6">
-        <f t="shared" ref="L48" si="13">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5">
+        <f t="shared" ref="L48" si="26">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>16.649999999999991</v>
       </c>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6">
-        <f t="shared" ref="N48" si="14">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5">
+        <f t="shared" ref="N48" si="27">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>14.979999999999992</v>
       </c>
-      <c r="O48" s="6"/>
-      <c r="P48" s="6">
-        <f t="shared" ref="P48" si="15">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5">
+        <f t="shared" ref="P48" si="28">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>13.309999999999992</v>
       </c>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6">
-        <f t="shared" ref="R48" si="16">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5">
+        <f t="shared" ref="R48" si="29">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>11.639999999999992</v>
       </c>
-      <c r="S48" s="6"/>
-      <c r="T48" s="6">
-        <f t="shared" ref="T48" si="17">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5">
+        <f t="shared" ref="T48" si="30">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>9.9699999999999918</v>
       </c>
-      <c r="U48" s="6"/>
-      <c r="V48" s="6">
-        <f t="shared" ref="V48" si="18">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5">
+        <f t="shared" ref="V48" si="31">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>8.2999999999999918</v>
       </c>
-      <c r="W48" s="6"/>
-      <c r="X48" s="6">
-        <f t="shared" ref="X48" si="19">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5">
+        <f t="shared" ref="X48" si="32">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>6.6299999999999919</v>
       </c>
-      <c r="Y48" s="6"/>
-      <c r="Z48" s="6">
-        <f t="shared" ref="Z48" si="20">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5">
+        <f t="shared" ref="Z48" si="33">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>4.959999999999992</v>
       </c>
-      <c r="AA48" s="6"/>
-      <c r="AB48" s="6">
-        <f t="shared" ref="AB48" si="21">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5">
+        <f t="shared" ref="AB48" si="34">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>3.289999999999992</v>
       </c>
-      <c r="AC48" s="6"/>
-      <c r="AD48" s="6">
-        <f t="shared" ref="AD48" si="22">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5">
+        <f t="shared" ref="AD48" si="35">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>1.6199999999999921</v>
       </c>
-      <c r="AE48" s="6"/>
+      <c r="AE48" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -4840,4 +5530,1256 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AE48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD47" sqref="AD47:AE47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>43061</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6">
+        <v>43062</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6">
+        <v>43063</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
+        <v>43064</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
+        <v>43065</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6">
+        <v>43066</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
+        <v>43067</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
+        <v>43068</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <v>43069</v>
+      </c>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6">
+        <v>43070</v>
+      </c>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
+        <v>43071</v>
+      </c>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6">
+        <v>43072</v>
+      </c>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6">
+        <v>43073</v>
+      </c>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6">
+        <v>43074</v>
+      </c>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6">
+        <v>43075</v>
+      </c>
+      <c r="AE5" s="6"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <f>SUM(C11:C45)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
+        <f>SUM(E11:E45)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7">
+        <f>SUM(G11:G45)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7">
+        <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7">
+        <f>SUM(K11:K45)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7">
+        <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
+        <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7">
+        <f>SUM(Q11:Q45)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7">
+        <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7">
+        <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7">
+        <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7">
+        <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7">
+        <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7">
+        <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7">
+        <f t="shared" ref="AD6" si="9">SUM(AE11:AE45)</f>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="7"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f>B3-(SUM(B6:AD6))</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AD11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AD12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AD13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AD14" s="3"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AD15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AD16" s="3"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AD17" s="3"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AD18" s="3"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AD19" s="3"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AD20" s="3"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AD22" s="3"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AD23" s="3"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AD24" s="3"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AD25" s="3"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AD26" s="3"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AD27" s="3"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AD28" s="3"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AD29" s="3"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AD30" s="3"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AD31" s="3"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AD32" s="3"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AD33" s="3"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AD34" s="3"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AD35" s="3"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AD36" s="3"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AD37" s="3"/>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AD38" s="3"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AD39" s="3"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AB40" s="3"/>
+      <c r="AD40" s="3"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AB41" s="3"/>
+      <c r="AD41" s="3"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AD42" s="3"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AD43" s="3"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AB44" s="3"/>
+      <c r="AD44" s="3"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AB45" s="3"/>
+      <c r="AD45" s="3"/>
+    </row>
+    <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="6">
+        <f>B5</f>
+        <v>43061</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6">
+        <f t="shared" ref="D46:AE46" si="10">D5</f>
+        <v>43062</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6">
+        <f t="shared" ref="F46:AE46" si="11">F5</f>
+        <v>43063</v>
+      </c>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
+        <f t="shared" ref="H46:AE46" si="12">H5</f>
+        <v>43064</v>
+      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6">
+        <f t="shared" ref="J46:AE46" si="13">J5</f>
+        <v>43065</v>
+      </c>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6">
+        <f t="shared" ref="L46:AE46" si="14">L5</f>
+        <v>43066</v>
+      </c>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6">
+        <f t="shared" ref="N46:AE46" si="15">N5</f>
+        <v>43067</v>
+      </c>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6">
+        <f t="shared" ref="P46:AE46" si="16">P5</f>
+        <v>43068</v>
+      </c>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6">
+        <f t="shared" ref="R46:AE46" si="17">R5</f>
+        <v>43069</v>
+      </c>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6">
+        <f t="shared" ref="T46:AE46" si="18">T5</f>
+        <v>43070</v>
+      </c>
+      <c r="U46" s="6"/>
+      <c r="V46" s="6">
+        <f t="shared" ref="V46:AE46" si="19">V5</f>
+        <v>43071</v>
+      </c>
+      <c r="W46" s="6"/>
+      <c r="X46" s="6">
+        <f t="shared" ref="X46:AE46" si="20">X5</f>
+        <v>43072</v>
+      </c>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6">
+        <f t="shared" ref="Z46:AE46" si="21">Z5</f>
+        <v>43073</v>
+      </c>
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6">
+        <f t="shared" ref="AB46:AE46" si="22">AB5</f>
+        <v>43074</v>
+      </c>
+      <c r="AC46" s="6"/>
+      <c r="AD46" s="6">
+        <f>AD5</f>
+        <v>43075</v>
+      </c>
+      <c r="AE46" s="6"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="5">
+        <f>$B$3-B6</f>
+        <v>25</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
+        <f>B47-D6</f>
+        <v>25</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
+        <f>D47-F6</f>
+        <v>25</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
+        <f>F47-H6</f>
+        <v>25</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
+        <f>H47-J6</f>
+        <v>25</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5">
+        <f>J47-L6</f>
+        <v>25</v>
+      </c>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5">
+        <f>L47-N6</f>
+        <v>25</v>
+      </c>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5">
+        <f>N47-P6</f>
+        <v>25</v>
+      </c>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5">
+        <f>P47-R6</f>
+        <v>25</v>
+      </c>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5">
+        <f>R47-T6</f>
+        <v>25</v>
+      </c>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5">
+        <f>T47-V6</f>
+        <v>25</v>
+      </c>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5">
+        <f>V47-X6</f>
+        <v>25</v>
+      </c>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5">
+        <f>X47-Z6</f>
+        <v>25</v>
+      </c>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5">
+        <f>Z47-AB6</f>
+        <v>25</v>
+      </c>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5">
+        <f>AB47-AD6</f>
+        <v>25</v>
+      </c>
+      <c r="AE47" s="5"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="5">
+        <f>B3</f>
+        <v>25</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
+        <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>23.33</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5">
+        <f t="shared" ref="F48" si="23">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>21.659999999999997</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5">
+        <f t="shared" ref="H48" si="24">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>19.989999999999995</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
+        <f t="shared" ref="J48" si="25">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>18.319999999999993</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5">
+        <f t="shared" ref="L48" si="26">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>16.649999999999991</v>
+      </c>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5">
+        <f t="shared" ref="N48" si="27">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>14.979999999999992</v>
+      </c>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5">
+        <f t="shared" ref="P48" si="28">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>13.309999999999992</v>
+      </c>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5">
+        <f t="shared" ref="R48" si="29">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>11.639999999999992</v>
+      </c>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5">
+        <f t="shared" ref="T48" si="30">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>9.9699999999999918</v>
+      </c>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5">
+        <f t="shared" ref="V48" si="31">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>8.2999999999999918</v>
+      </c>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5">
+        <f t="shared" ref="X48" si="32">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>6.6299999999999919</v>
+      </c>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5">
+        <f t="shared" ref="Z48" si="33">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>4.959999999999992</v>
+      </c>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5">
+        <f t="shared" ref="AB48" si="34">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>3.289999999999992</v>
+      </c>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5">
+        <f t="shared" ref="AD48" si="35">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>1.6199999999999921</v>
+      </c>
+      <c r="AE48" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="76">
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Z46:AA46"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="A10:A45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="AD46:AE46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="T46:U46"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="X46:Y46"/>
+    <mergeCell ref="AD48:AE48"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="X48:Y48"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="AB48:AC48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#45 added to burndown chart
</commit_message>
<xml_diff>
--- a/planning/BurndownChart.xlsx
+++ b/planning/BurndownChart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 Burndown Chart" sheetId="2" r:id="rId1"/>
@@ -153,17 +153,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,43 +1007,43 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2988,7 +2988,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -3041,146 +3041,146 @@
       </c>
     </row>
     <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>43061</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
         <v>43062</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
         <v>43063</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
         <v>43064</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
         <v>43065</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5">
         <v>43066</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6">
+      <c r="M5" s="5"/>
+      <c r="N5" s="5">
         <v>43067</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
         <v>43068</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5">
         <v>43069</v>
       </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6">
+      <c r="S5" s="5"/>
+      <c r="T5" s="5">
         <v>43070</v>
       </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6">
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
         <v>43071</v>
       </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6">
+      <c r="W5" s="5"/>
+      <c r="X5" s="5">
         <v>43072</v>
       </c>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6">
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5">
         <v>43073</v>
       </c>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6">
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5">
         <v>43074</v>
       </c>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6">
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5">
         <v>43075</v>
       </c>
-      <c r="AE5" s="6"/>
+      <c r="AE5" s="5"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="4">
         <f>SUM(C11:C45)</f>
         <v>2</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
         <f>SUM(E11:E45)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
         <f>SUM(G11:G45)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
         <v>1</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
         <f>SUM(K11:K45)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4">
         <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4">
         <f>SUM(Q11:Q45)</f>
         <v>10</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4">
         <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7">
+      <c r="S6" s="4"/>
+      <c r="T6" s="4">
         <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4">
         <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7">
+      <c r="W6" s="4"/>
+      <c r="X6" s="4">
         <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7">
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4">
         <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7">
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4">
         <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
         <v>1</v>
       </c>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7">
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4">
         <f>SUM(AE11:AE45)</f>
         <v>21</v>
       </c>
-      <c r="AE6" s="7"/>
+      <c r="AE6" s="4"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -3192,7 +3192,7 @@
       </c>
     </row>
     <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -3287,7 +3287,7 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="3">
         <v>12</v>
       </c>
@@ -3330,7 +3330,7 @@
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3">
         <v>13</v>
       </c>
@@ -3362,7 +3362,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
@@ -3390,7 +3390,7 @@
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -3418,7 +3418,7 @@
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -3440,7 +3440,7 @@
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
@@ -3463,7 +3463,7 @@
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
@@ -3486,7 +3486,7 @@
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
@@ -3504,7 +3504,7 @@
       <c r="AD18" s="3"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="7"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
       <c r="H19" s="3"/>
@@ -3521,7 +3521,7 @@
       <c r="AD19" s="3"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="7"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
       <c r="H20" s="3"/>
@@ -3538,7 +3538,7 @@
       <c r="AD20" s="3"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
@@ -3556,7 +3556,7 @@
       <c r="AD21" s="3"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
@@ -3574,7 +3574,7 @@
       <c r="AD22" s="3"/>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
@@ -3592,7 +3592,7 @@
       <c r="AD23" s="3"/>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
@@ -3610,7 +3610,7 @@
       <c r="AD24" s="3"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
@@ -3628,7 +3628,7 @@
       <c r="AD25" s="3"/>
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
@@ -3646,7 +3646,7 @@
       <c r="AD26" s="3"/>
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
@@ -3664,7 +3664,7 @@
       <c r="AD27" s="3"/>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
@@ -3682,7 +3682,7 @@
       <c r="AD28" s="3"/>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
@@ -3700,7 +3700,7 @@
       <c r="AD29" s="3"/>
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
@@ -3718,7 +3718,7 @@
       <c r="AD30" s="3"/>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
@@ -3736,7 +3736,7 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
@@ -3754,7 +3754,7 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
@@ -3772,7 +3772,7 @@
       <c r="AD33" s="3"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
@@ -3790,7 +3790,7 @@
       <c r="AD34" s="3"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
@@ -3808,7 +3808,7 @@
       <c r="AD35" s="3"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
@@ -3826,7 +3826,7 @@
       <c r="AD36" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
@@ -3844,7 +3844,7 @@
       <c r="AD37" s="3"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
@@ -3862,7 +3862,7 @@
       <c r="AD38" s="3"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
@@ -3880,7 +3880,7 @@
       <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
@@ -3898,7 +3898,7 @@
       <c r="AD40" s="3"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
@@ -3916,7 +3916,7 @@
       <c r="AD41" s="3"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
@@ -3934,7 +3934,7 @@
       <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
@@ -3952,7 +3952,7 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
@@ -3970,7 +3970,7 @@
       <c r="AD44" s="3"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
@@ -3988,222 +3988,268 @@
       <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <v>43061</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5">
         <v>43062</v>
       </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6">
+      <c r="E46" s="5"/>
+      <c r="F46" s="5">
         <v>43063</v>
       </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6">
+      <c r="G46" s="5"/>
+      <c r="H46" s="5">
         <v>43064</v>
       </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6">
+      <c r="I46" s="5"/>
+      <c r="J46" s="5">
         <v>43065</v>
       </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6">
+      <c r="K46" s="5"/>
+      <c r="L46" s="5">
         <v>43066</v>
       </c>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6">
+      <c r="M46" s="5"/>
+      <c r="N46" s="5">
         <v>43067</v>
       </c>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6">
+      <c r="O46" s="5"/>
+      <c r="P46" s="5">
         <v>43068</v>
       </c>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6">
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5">
         <v>43069</v>
       </c>
-      <c r="S46" s="6"/>
-      <c r="T46" s="6">
+      <c r="S46" s="5"/>
+      <c r="T46" s="5">
         <v>43070</v>
       </c>
-      <c r="U46" s="6"/>
-      <c r="V46" s="6">
+      <c r="U46" s="5"/>
+      <c r="V46" s="5">
         <v>43071</v>
       </c>
-      <c r="W46" s="6"/>
-      <c r="X46" s="6">
+      <c r="W46" s="5"/>
+      <c r="X46" s="5">
         <v>43072</v>
       </c>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6">
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5">
         <v>43073</v>
       </c>
-      <c r="AA46" s="6"/>
-      <c r="AB46" s="6">
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5">
         <v>43074</v>
       </c>
-      <c r="AC46" s="6"/>
-      <c r="AD46" s="6">
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5">
         <v>43075</v>
       </c>
-      <c r="AE46" s="6"/>
+      <c r="AE46" s="5"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <f>$B$3-B6</f>
         <v>33</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6">
         <f>B47-D6</f>
         <v>33</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5">
+      <c r="E47" s="6"/>
+      <c r="F47" s="6">
         <f>D47-F6</f>
         <v>33</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6">
         <f>F47-H6</f>
         <v>32</v>
       </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5">
+      <c r="I47" s="6"/>
+      <c r="J47" s="6">
         <f>H47-J6</f>
         <v>32</v>
       </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5">
+      <c r="K47" s="6"/>
+      <c r="L47" s="6">
         <f>J47-L6</f>
         <v>32</v>
       </c>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5">
+      <c r="M47" s="6"/>
+      <c r="N47" s="6">
         <f>L47-N6</f>
         <v>32</v>
       </c>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5">
+      <c r="O47" s="6"/>
+      <c r="P47" s="6">
         <f>N47-P6</f>
         <v>22</v>
       </c>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5">
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6">
         <f>P47-R6</f>
         <v>22</v>
       </c>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5">
+      <c r="S47" s="6"/>
+      <c r="T47" s="6">
         <f>R47-T6</f>
         <v>22</v>
       </c>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5">
+      <c r="U47" s="6"/>
+      <c r="V47" s="6">
         <f>T47-V6</f>
         <v>22</v>
       </c>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5">
+      <c r="W47" s="6"/>
+      <c r="X47" s="6">
         <f>V47-X6</f>
         <v>22</v>
       </c>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5">
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6">
         <f>X47-Z6</f>
         <v>22</v>
       </c>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="5">
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6">
         <f>Z47-AB6</f>
         <v>21</v>
       </c>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5">
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6">
         <f>AB47-AD6</f>
         <v>0</v>
       </c>
-      <c r="AE47" s="5"/>
+      <c r="AE47" s="6"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <f>B3</f>
         <v>35</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6">
         <v>32.5</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5">
+      <c r="E48" s="6"/>
+      <c r="F48" s="6">
         <v>30</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5">
+      <c r="G48" s="6"/>
+      <c r="H48" s="6">
         <v>27.5</v>
       </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5">
+      <c r="I48" s="6"/>
+      <c r="J48" s="6">
         <v>25</v>
       </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5">
+      <c r="K48" s="6"/>
+      <c r="L48" s="6">
         <v>22</v>
       </c>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5">
+      <c r="M48" s="6"/>
+      <c r="N48" s="6">
         <v>19.5</v>
       </c>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5">
+      <c r="O48" s="6"/>
+      <c r="P48" s="6">
         <v>17</v>
       </c>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5">
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6">
         <v>14.5</v>
       </c>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5">
+      <c r="S48" s="6"/>
+      <c r="T48" s="6">
         <v>12</v>
       </c>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5">
+      <c r="U48" s="6"/>
+      <c r="V48" s="6">
         <v>9.5</v>
       </c>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5">
+      <c r="W48" s="6"/>
+      <c r="X48" s="6">
         <v>7</v>
       </c>
-      <c r="Y48" s="5"/>
-      <c r="Z48" s="5">
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6">
         <v>4.5</v>
       </c>
-      <c r="AA48" s="5"/>
-      <c r="AB48" s="5">
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6">
         <v>2</v>
       </c>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5">
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6">
         <v>0</v>
       </c>
-      <c r="AE48" s="5"/>
+      <c r="AE48" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="76">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="A10:A45"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="T46:U46"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="Z46:AA46"/>
+    <mergeCell ref="X48:Y48"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="X46:Y46"/>
+    <mergeCell ref="AD46:AE46"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="AD48:AE48"/>
+    <mergeCell ref="AB48:AC48"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="F46:G46"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="H46:I46"/>
@@ -4220,59 +4266,13 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="AB46:AC46"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="A10:A45"/>
-    <mergeCell ref="T48:U48"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="T46:U46"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="Z48:AA48"/>
-    <mergeCell ref="Z47:AA47"/>
-    <mergeCell ref="Z46:AA46"/>
-    <mergeCell ref="X48:Y48"/>
-    <mergeCell ref="X47:Y47"/>
-    <mergeCell ref="X46:Y46"/>
-    <mergeCell ref="AD46:AE46"/>
-    <mergeCell ref="AD47:AE47"/>
-    <mergeCell ref="AD48:AE48"/>
-    <mergeCell ref="AB48:AC48"/>
-    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="P6:Q6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
@@ -4284,8 +4284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE7739D-713E-4D3F-8C3C-20CB148605F1}">
   <dimension ref="A1:AE48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4337,146 +4337,146 @@
       </c>
     </row>
     <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>43075</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
         <v>43076</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
         <v>43077</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
         <v>43078</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
         <v>43079</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6">
+      <c r="K5" s="5"/>
+      <c r="L5" s="5">
         <v>43080</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6">
+      <c r="M5" s="5"/>
+      <c r="N5" s="5">
         <v>43081</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6">
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
         <v>43082</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5">
         <v>43083</v>
       </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6">
+      <c r="S5" s="5"/>
+      <c r="T5" s="5">
         <v>43084</v>
       </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6">
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
         <v>43085</v>
       </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6">
+      <c r="W5" s="5"/>
+      <c r="X5" s="5">
         <v>43086</v>
       </c>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6">
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5">
         <v>43087</v>
       </c>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6">
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5">
         <v>43088</v>
       </c>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6">
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5">
         <v>43089</v>
       </c>
-      <c r="AE5" s="6"/>
+      <c r="AE5" s="5"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="4">
         <f>SUM(C11:C45)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7">
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
         <f>SUM(E11:E45)</f>
         <v>0</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
         <f>SUM(G11:G45)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
         <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
         <f>SUM(K11:K45)</f>
         <v>0</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7">
+      <c r="M6" s="4"/>
+      <c r="N6" s="4">
         <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4">
         <f>SUM(Q11:Q45)</f>
         <v>0</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4">
         <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
         <v>0</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7">
+      <c r="S6" s="4"/>
+      <c r="T6" s="4">
         <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
         <v>0</v>
       </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7">
+      <c r="U6" s="4"/>
+      <c r="V6" s="4">
         <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7">
+      <c r="W6" s="4"/>
+      <c r="X6" s="4">
         <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7">
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4">
         <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7">
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4">
         <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
         <v>0</v>
       </c>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7">
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4">
         <f t="shared" ref="AD6" si="9">SUM(AE11:AE45)</f>
         <v>0</v>
       </c>
-      <c r="AE6" s="7"/>
+      <c r="AE6" s="4"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -4484,11 +4484,11 @@
       </c>
       <c r="B8">
         <f>B3-(SUM(B6:AD6))</f>
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4583,7 +4583,1264 @@
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="F11" s="3">
+        <v>45</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AD11" s="3"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="V12" s="3"/>
+      <c r="X12" s="3"/>
+      <c r="Z12" s="3"/>
+      <c r="AB12" s="3"/>
+      <c r="AD12" s="3"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="V13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Z13" s="3"/>
+      <c r="AB13" s="3"/>
+      <c r="AD13" s="3"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AD14" s="3"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="V15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AD15" s="3"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="T16" s="3"/>
+      <c r="V16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AD16" s="3"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AD17" s="3"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="T18" s="3"/>
+      <c r="V18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AD18" s="3"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="T19" s="3"/>
+      <c r="V19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AD19" s="3"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Z20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AD20" s="3"/>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Z21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="T22" s="3"/>
+      <c r="V22" s="3"/>
+      <c r="X22" s="3"/>
+      <c r="Z22" s="3"/>
+      <c r="AB22" s="3"/>
+      <c r="AD22" s="3"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AD23" s="3"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AD24" s="3"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A25" s="7"/>
+      <c r="B25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AD25" s="3"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AD26" s="3"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AD27" s="3"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A28" s="7"/>
+      <c r="B28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="T28" s="3"/>
+      <c r="V28" s="3"/>
+      <c r="X28" s="3"/>
+      <c r="Z28" s="3"/>
+      <c r="AB28" s="3"/>
+      <c r="AD28" s="3"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="T29" s="3"/>
+      <c r="V29" s="3"/>
+      <c r="X29" s="3"/>
+      <c r="Z29" s="3"/>
+      <c r="AB29" s="3"/>
+      <c r="AD29" s="3"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="T30" s="3"/>
+      <c r="V30" s="3"/>
+      <c r="X30" s="3"/>
+      <c r="Z30" s="3"/>
+      <c r="AB30" s="3"/>
+      <c r="AD30" s="3"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AD31" s="3"/>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="T32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AD32" s="3"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="T33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AD33" s="3"/>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="T34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AD34" s="3"/>
+    </row>
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="T35" s="3"/>
+      <c r="V35" s="3"/>
+      <c r="X35" s="3"/>
+      <c r="Z35" s="3"/>
+      <c r="AB35" s="3"/>
+      <c r="AD35" s="3"/>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="T36" s="3"/>
+      <c r="V36" s="3"/>
+      <c r="X36" s="3"/>
+      <c r="Z36" s="3"/>
+      <c r="AB36" s="3"/>
+      <c r="AD36" s="3"/>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="T37" s="3"/>
+      <c r="V37" s="3"/>
+      <c r="X37" s="3"/>
+      <c r="Z37" s="3"/>
+      <c r="AB37" s="3"/>
+      <c r="AD37" s="3"/>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="T38" s="3"/>
+      <c r="V38" s="3"/>
+      <c r="X38" s="3"/>
+      <c r="Z38" s="3"/>
+      <c r="AB38" s="3"/>
+      <c r="AD38" s="3"/>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="T39" s="3"/>
+      <c r="V39" s="3"/>
+      <c r="X39" s="3"/>
+      <c r="Z39" s="3"/>
+      <c r="AB39" s="3"/>
+      <c r="AD39" s="3"/>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="T40" s="3"/>
+      <c r="V40" s="3"/>
+      <c r="X40" s="3"/>
+      <c r="Z40" s="3"/>
+      <c r="AB40" s="3"/>
+      <c r="AD40" s="3"/>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="T41" s="3"/>
+      <c r="V41" s="3"/>
+      <c r="X41" s="3"/>
+      <c r="Z41" s="3"/>
+      <c r="AB41" s="3"/>
+      <c r="AD41" s="3"/>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="X42" s="3"/>
+      <c r="Z42" s="3"/>
+      <c r="AB42" s="3"/>
+      <c r="AD42" s="3"/>
+    </row>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="X43" s="3"/>
+      <c r="Z43" s="3"/>
+      <c r="AB43" s="3"/>
+      <c r="AD43" s="3"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="T44" s="3"/>
+      <c r="V44" s="3"/>
+      <c r="X44" s="3"/>
+      <c r="Z44" s="3"/>
+      <c r="AB44" s="3"/>
+      <c r="AD44" s="3"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="T45" s="3"/>
+      <c r="V45" s="3"/>
+      <c r="X45" s="3"/>
+      <c r="Z45" s="3"/>
+      <c r="AB45" s="3"/>
+      <c r="AD45" s="3"/>
+    </row>
+    <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="5">
+        <f>B5</f>
+        <v>43075</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5">
+        <f t="shared" ref="D46" si="10">D5</f>
+        <v>43076</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5">
+        <f t="shared" ref="F46" si="11">F5</f>
+        <v>43077</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5">
+        <f t="shared" ref="H46" si="12">H5</f>
+        <v>43078</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5">
+        <f t="shared" ref="J46" si="13">J5</f>
+        <v>43079</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5">
+        <f t="shared" ref="L46" si="14">L5</f>
+        <v>43080</v>
+      </c>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5">
+        <f t="shared" ref="N46" si="15">N5</f>
+        <v>43081</v>
+      </c>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5">
+        <f t="shared" ref="P46" si="16">P5</f>
+        <v>43082</v>
+      </c>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5">
+        <f t="shared" ref="R46" si="17">R5</f>
+        <v>43083</v>
+      </c>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5">
+        <f t="shared" ref="T46" si="18">T5</f>
+        <v>43084</v>
+      </c>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5">
+        <f t="shared" ref="V46" si="19">V5</f>
+        <v>43085</v>
+      </c>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5">
+        <f t="shared" ref="X46" si="20">X5</f>
+        <v>43086</v>
+      </c>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5">
+        <f t="shared" ref="Z46" si="21">Z5</f>
+        <v>43087</v>
+      </c>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5">
+        <f t="shared" ref="AB46" si="22">AB5</f>
+        <v>43088</v>
+      </c>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5">
+        <f>AD5</f>
+        <v>43089</v>
+      </c>
+      <c r="AE46" s="5"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="6">
+        <f>$B$3-B6</f>
+        <v>25</v>
+      </c>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6">
+        <f>B47-D6</f>
+        <v>25</v>
+      </c>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6">
+        <f>D47-F6</f>
+        <v>23</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6">
+        <f>F47-H6</f>
+        <v>23</v>
+      </c>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6">
+        <f>H47-J6</f>
+        <v>23</v>
+      </c>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6">
+        <f>J47-L6</f>
+        <v>23</v>
+      </c>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6">
+        <f>L47-N6</f>
+        <v>23</v>
+      </c>
+      <c r="O47" s="6"/>
+      <c r="P47" s="6">
+        <f>N47-P6</f>
+        <v>23</v>
+      </c>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6">
+        <f>P47-R6</f>
+        <v>23</v>
+      </c>
+      <c r="S47" s="6"/>
+      <c r="T47" s="6">
+        <f>R47-T6</f>
+        <v>23</v>
+      </c>
+      <c r="U47" s="6"/>
+      <c r="V47" s="6">
+        <f>T47-V6</f>
+        <v>23</v>
+      </c>
+      <c r="W47" s="6"/>
+      <c r="X47" s="6">
+        <f>V47-X6</f>
+        <v>23</v>
+      </c>
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6">
+        <f>X47-Z6</f>
+        <v>23</v>
+      </c>
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6">
+        <f>Z47-AB6</f>
+        <v>23</v>
+      </c>
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6">
+        <f>AB47-AD6</f>
+        <v>23</v>
+      </c>
+      <c r="AE47" s="6"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="6">
+        <f>B3</f>
+        <v>25</v>
+      </c>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6">
+        <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>23.33</v>
+      </c>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6">
+        <f t="shared" ref="F48" si="23">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>21.659999999999997</v>
+      </c>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6">
+        <f t="shared" ref="H48" si="24">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>19.989999999999995</v>
+      </c>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6">
+        <f t="shared" ref="J48" si="25">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>18.319999999999993</v>
+      </c>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6">
+        <f t="shared" ref="L48" si="26">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>16.649999999999991</v>
+      </c>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6">
+        <f t="shared" ref="N48" si="27">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>14.979999999999992</v>
+      </c>
+      <c r="O48" s="6"/>
+      <c r="P48" s="6">
+        <f t="shared" ref="P48" si="28">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>13.309999999999992</v>
+      </c>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6">
+        <f t="shared" ref="R48" si="29">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>11.639999999999992</v>
+      </c>
+      <c r="S48" s="6"/>
+      <c r="T48" s="6">
+        <f t="shared" ref="T48" si="30">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>9.9699999999999918</v>
+      </c>
+      <c r="U48" s="6"/>
+      <c r="V48" s="6">
+        <f t="shared" ref="V48" si="31">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>8.2999999999999918</v>
+      </c>
+      <c r="W48" s="6"/>
+      <c r="X48" s="6">
+        <f t="shared" ref="X48" si="32">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>6.6299999999999919</v>
+      </c>
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6">
+        <f t="shared" ref="Z48" si="33">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>4.959999999999992</v>
+      </c>
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6">
+        <f t="shared" ref="AB48" si="34">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>3.289999999999992</v>
+      </c>
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6">
+        <f t="shared" ref="AD48" si="35">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
+        <v>1.6199999999999921</v>
+      </c>
+      <c r="AE48" s="6"/>
+    </row>
+  </sheetData>
+  <mergeCells count="76">
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="Z46:AA46"/>
+    <mergeCell ref="AB6:AC6"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="A10:A45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="T6:U6"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="X6:Y6"/>
+    <mergeCell ref="AB47:AC47"/>
+    <mergeCell ref="AB46:AC46"/>
+    <mergeCell ref="AD46:AE46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="R46:S46"/>
+    <mergeCell ref="T46:U46"/>
+    <mergeCell ref="V46:W46"/>
+    <mergeCell ref="X46:Y46"/>
+    <mergeCell ref="AD48:AE48"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="R48:S48"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="T47:U47"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="X47:Y47"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="V48:W48"/>
+    <mergeCell ref="X48:Y48"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="AB48:AC48"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AE48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AD47" sqref="AD47:AE47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
+        <v>43061</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>43062</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <v>43063</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
+        <v>43064</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
+        <v>43065</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5">
+        <v>43066</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5">
+        <v>43067</v>
+      </c>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5">
+        <v>43068</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5">
+        <v>43069</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5">
+        <v>43070</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
+        <v>43071</v>
+      </c>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5">
+        <v>43072</v>
+      </c>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5">
+        <v>43073</v>
+      </c>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5">
+        <v>43074</v>
+      </c>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5">
+        <v>43075</v>
+      </c>
+      <c r="AE5" s="5"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <f>SUM(C11:C45)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <f>SUM(E11:E45)</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <f>SUM(G11:G45)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
+        <f>SUM(K11:K45)</f>
+        <v>0</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4">
+        <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4">
+        <f>SUM(Q11:Q45)</f>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4">
+        <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
+        <v>0</v>
+      </c>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4">
+        <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4">
+        <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
+        <v>0</v>
+      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4">
+        <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
+        <v>0</v>
+      </c>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4">
+        <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
+        <v>0</v>
+      </c>
+      <c r="AA6" s="4"/>
+      <c r="AB6" s="4">
+        <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
+        <v>0</v>
+      </c>
+      <c r="AC6" s="4"/>
+      <c r="AD6" s="4">
+        <f t="shared" ref="AD6" si="9">SUM(AE11:AE45)</f>
+        <v>0</v>
+      </c>
+      <c r="AE6" s="4"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <f>B3-(SUM(B6:AD6))</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
       <c r="B11" s="3"/>
       <c r="D11" s="3"/>
       <c r="F11" s="3"/>
@@ -4601,7 +5858,7 @@
       <c r="AD11" s="3"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="3"/>
@@ -4619,7 +5876,7 @@
       <c r="AD12" s="3"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
@@ -4637,7 +5894,7 @@
       <c r="AD13" s="3"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -4655,7 +5912,7 @@
       <c r="AD14" s="3"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -4672,7 +5929,7 @@
       <c r="AD15" s="3"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="3"/>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
@@ -4690,7 +5947,7 @@
       <c r="AD16" s="3"/>
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
@@ -4708,7 +5965,7 @@
       <c r="AD17" s="3"/>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
@@ -4726,7 +5983,7 @@
       <c r="AD18" s="3"/>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="F19" s="3"/>
@@ -4744,7 +6001,7 @@
       <c r="AD19" s="3"/>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
@@ -4762,7 +6019,7 @@
       <c r="AD20" s="3"/>
     </row>
     <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="3"/>
       <c r="D21" s="3"/>
       <c r="F21" s="3"/>
@@ -4780,7 +6037,7 @@
       <c r="AD21" s="3"/>
     </row>
     <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="3"/>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
@@ -4798,7 +6055,7 @@
       <c r="AD22" s="3"/>
     </row>
     <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
@@ -4816,7 +6073,7 @@
       <c r="AD23" s="3"/>
     </row>
     <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="3"/>
       <c r="D24" s="3"/>
       <c r="F24" s="3"/>
@@ -4834,7 +6091,7 @@
       <c r="AD24" s="3"/>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="D25" s="3"/>
       <c r="F25" s="3"/>
@@ -4852,7 +6109,7 @@
       <c r="AD25" s="3"/>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="D26" s="3"/>
       <c r="F26" s="3"/>
@@ -4870,7 +6127,7 @@
       <c r="AD26" s="3"/>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="3"/>
       <c r="D27" s="3"/>
       <c r="F27" s="3"/>
@@ -4888,7 +6145,7 @@
       <c r="AD27" s="3"/>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3"/>
       <c r="D28" s="3"/>
       <c r="F28" s="3"/>
@@ -4906,7 +6163,7 @@
       <c r="AD28" s="3"/>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
@@ -4924,7 +6181,7 @@
       <c r="AD29" s="3"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="3"/>
       <c r="D30" s="3"/>
       <c r="F30" s="3"/>
@@ -4942,7 +6199,7 @@
       <c r="AD30" s="3"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="3"/>
       <c r="D31" s="3"/>
       <c r="F31" s="3"/>
@@ -4960,7 +6217,7 @@
       <c r="AD31" s="3"/>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="3"/>
       <c r="D32" s="3"/>
       <c r="F32" s="3"/>
@@ -4978,7 +6235,7 @@
       <c r="AD32" s="3"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="D33" s="3"/>
       <c r="F33" s="3"/>
@@ -4996,7 +6253,7 @@
       <c r="AD33" s="3"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="3"/>
       <c r="D34" s="3"/>
       <c r="F34" s="3"/>
@@ -5014,7 +6271,7 @@
       <c r="AD34" s="3"/>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="3"/>
       <c r="D35" s="3"/>
       <c r="F35" s="3"/>
@@ -5032,7 +6289,7 @@
       <c r="AD35" s="3"/>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="3"/>
       <c r="D36" s="3"/>
       <c r="F36" s="3"/>
@@ -5050,7 +6307,7 @@
       <c r="AD36" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="3"/>
       <c r="D37" s="3"/>
       <c r="F37" s="3"/>
@@ -5068,7 +6325,7 @@
       <c r="AD37" s="3"/>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="3"/>
       <c r="D38" s="3"/>
       <c r="F38" s="3"/>
@@ -5086,7 +6343,7 @@
       <c r="AD38" s="3"/>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="3"/>
       <c r="D39" s="3"/>
       <c r="F39" s="3"/>
@@ -5104,7 +6361,7 @@
       <c r="AD39" s="3"/>
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="3"/>
       <c r="D40" s="3"/>
       <c r="F40" s="3"/>
@@ -5122,7 +6379,7 @@
       <c r="AD40" s="3"/>
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="3"/>
       <c r="D41" s="3"/>
       <c r="F41" s="3"/>
@@ -5140,7 +6397,7 @@
       <c r="AD41" s="3"/>
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="3"/>
       <c r="D42" s="3"/>
       <c r="F42" s="3"/>
@@ -5158,7 +6415,7 @@
       <c r="AD42" s="3"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="3"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
@@ -5176,7 +6433,7 @@
       <c r="AD43" s="3"/>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="3"/>
       <c r="D44" s="3"/>
       <c r="F44" s="3"/>
@@ -5194,7 +6451,7 @@
       <c r="AD44" s="3"/>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="3"/>
       <c r="D45" s="3"/>
       <c r="F45" s="3"/>
@@ -5212,241 +6469,241 @@
       <c r="AD45" s="3"/>
     </row>
     <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="6">
+      <c r="B46" s="5">
         <f>B5</f>
+        <v>43061</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5">
+        <f t="shared" ref="D46" si="10">D5</f>
+        <v>43062</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5">
+        <f t="shared" ref="F46" si="11">F5</f>
+        <v>43063</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5">
+        <f t="shared" ref="H46" si="12">H5</f>
+        <v>43064</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5">
+        <f t="shared" ref="J46" si="13">J5</f>
+        <v>43065</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5">
+        <f t="shared" ref="L46" si="14">L5</f>
+        <v>43066</v>
+      </c>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5">
+        <f t="shared" ref="N46" si="15">N5</f>
+        <v>43067</v>
+      </c>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5">
+        <f t="shared" ref="P46" si="16">P5</f>
+        <v>43068</v>
+      </c>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5">
+        <f t="shared" ref="R46" si="17">R5</f>
+        <v>43069</v>
+      </c>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5">
+        <f t="shared" ref="T46" si="18">T5</f>
+        <v>43070</v>
+      </c>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5">
+        <f t="shared" ref="V46" si="19">V5</f>
+        <v>43071</v>
+      </c>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5">
+        <f t="shared" ref="X46" si="20">X5</f>
+        <v>43072</v>
+      </c>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5">
+        <f t="shared" ref="Z46" si="21">Z5</f>
+        <v>43073</v>
+      </c>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5">
+        <f t="shared" ref="AB46" si="22">AB5</f>
+        <v>43074</v>
+      </c>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5">
+        <f>AD5</f>
         <v>43075</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6">
-        <f t="shared" ref="D46:AE46" si="10">D5</f>
-        <v>43076</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6">
-        <f t="shared" ref="F46:AE46" si="11">F5</f>
-        <v>43077</v>
-      </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6">
-        <f t="shared" ref="H46:AE46" si="12">H5</f>
-        <v>43078</v>
-      </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6">
-        <f t="shared" ref="J46:AE46" si="13">J5</f>
-        <v>43079</v>
-      </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6">
-        <f t="shared" ref="L46:AE46" si="14">L5</f>
-        <v>43080</v>
-      </c>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6">
-        <f t="shared" ref="N46:AE46" si="15">N5</f>
-        <v>43081</v>
-      </c>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6">
-        <f t="shared" ref="P46:AE46" si="16">P5</f>
-        <v>43082</v>
-      </c>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6">
-        <f t="shared" ref="R46:AE46" si="17">R5</f>
-        <v>43083</v>
-      </c>
-      <c r="S46" s="6"/>
-      <c r="T46" s="6">
-        <f t="shared" ref="T46:AE46" si="18">T5</f>
-        <v>43084</v>
-      </c>
-      <c r="U46" s="6"/>
-      <c r="V46" s="6">
-        <f t="shared" ref="V46:AE46" si="19">V5</f>
-        <v>43085</v>
-      </c>
-      <c r="W46" s="6"/>
-      <c r="X46" s="6">
-        <f t="shared" ref="X46:AE46" si="20">X5</f>
-        <v>43086</v>
-      </c>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6">
-        <f t="shared" ref="Z46:AE46" si="21">Z5</f>
-        <v>43087</v>
-      </c>
-      <c r="AA46" s="6"/>
-      <c r="AB46" s="6">
-        <f t="shared" ref="AB46:AE46" si="22">AB5</f>
-        <v>43088</v>
-      </c>
-      <c r="AC46" s="6"/>
-      <c r="AD46" s="6">
-        <f>AD5</f>
-        <v>43089</v>
-      </c>
-      <c r="AE46" s="6"/>
+      <c r="AE46" s="5"/>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="6">
         <f>$B$3-B6</f>
         <v>25</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6">
         <f>B47-D6</f>
         <v>25</v>
       </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5">
+      <c r="E47" s="6"/>
+      <c r="F47" s="6">
         <f>D47-F6</f>
         <v>25</v>
       </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5">
+      <c r="G47" s="6"/>
+      <c r="H47" s="6">
         <f>F47-H6</f>
         <v>25</v>
       </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5">
+      <c r="I47" s="6"/>
+      <c r="J47" s="6">
         <f>H47-J6</f>
         <v>25</v>
       </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5">
+      <c r="K47" s="6"/>
+      <c r="L47" s="6">
         <f>J47-L6</f>
         <v>25</v>
       </c>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5">
+      <c r="M47" s="6"/>
+      <c r="N47" s="6">
         <f>L47-N6</f>
         <v>25</v>
       </c>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5">
+      <c r="O47" s="6"/>
+      <c r="P47" s="6">
         <f>N47-P6</f>
         <v>25</v>
       </c>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5">
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6">
         <f>P47-R6</f>
         <v>25</v>
       </c>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5">
+      <c r="S47" s="6"/>
+      <c r="T47" s="6">
         <f>R47-T6</f>
         <v>25</v>
       </c>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5">
+      <c r="U47" s="6"/>
+      <c r="V47" s="6">
         <f>T47-V6</f>
         <v>25</v>
       </c>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5">
+      <c r="W47" s="6"/>
+      <c r="X47" s="6">
         <f>V47-X6</f>
         <v>25</v>
       </c>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5">
+      <c r="Y47" s="6"/>
+      <c r="Z47" s="6">
         <f>X47-Z6</f>
         <v>25</v>
       </c>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="5">
+      <c r="AA47" s="6"/>
+      <c r="AB47" s="6">
         <f>Z47-AB6</f>
         <v>25</v>
       </c>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5">
+      <c r="AC47" s="6"/>
+      <c r="AD47" s="6">
         <f>AB47-AD6</f>
         <v>25</v>
       </c>
-      <c r="AE47" s="5"/>
+      <c r="AE47" s="6"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B48" s="5">
+      <c r="B48" s="6">
         <f>B3</f>
         <v>25</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6">
         <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>23.33</v>
       </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5">
+      <c r="E48" s="6"/>
+      <c r="F48" s="6">
         <f t="shared" ref="F48" si="23">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>21.659999999999997</v>
       </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5">
+      <c r="G48" s="6"/>
+      <c r="H48" s="6">
         <f t="shared" ref="H48" si="24">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>19.989999999999995</v>
       </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5">
+      <c r="I48" s="6"/>
+      <c r="J48" s="6">
         <f t="shared" ref="J48" si="25">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>18.319999999999993</v>
       </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5">
+      <c r="K48" s="6"/>
+      <c r="L48" s="6">
         <f t="shared" ref="L48" si="26">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>16.649999999999991</v>
       </c>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5">
+      <c r="M48" s="6"/>
+      <c r="N48" s="6">
         <f t="shared" ref="N48" si="27">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>14.979999999999992</v>
       </c>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5">
+      <c r="O48" s="6"/>
+      <c r="P48" s="6">
         <f t="shared" ref="P48" si="28">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>13.309999999999992</v>
       </c>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5">
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6">
         <f t="shared" ref="R48" si="29">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>11.639999999999992</v>
       </c>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5">
+      <c r="S48" s="6"/>
+      <c r="T48" s="6">
         <f t="shared" ref="T48" si="30">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>9.9699999999999918</v>
       </c>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5">
+      <c r="U48" s="6"/>
+      <c r="V48" s="6">
         <f t="shared" ref="V48" si="31">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>8.2999999999999918</v>
       </c>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5">
+      <c r="W48" s="6"/>
+      <c r="X48" s="6">
         <f t="shared" ref="X48" si="32">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>6.6299999999999919</v>
       </c>
-      <c r="Y48" s="5"/>
-      <c r="Z48" s="5">
+      <c r="Y48" s="6"/>
+      <c r="Z48" s="6">
         <f t="shared" ref="Z48" si="33">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>4.959999999999992</v>
       </c>
-      <c r="AA48" s="5"/>
-      <c r="AB48" s="5">
+      <c r="AA48" s="6"/>
+      <c r="AB48" s="6">
         <f t="shared" ref="AB48" si="34">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>3.289999999999992</v>
       </c>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5">
+      <c r="AC48" s="6"/>
+      <c r="AD48" s="6">
         <f t="shared" ref="AD48" si="35">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
         <v>1.6199999999999921</v>
       </c>
-      <c r="AE48" s="5"/>
+      <c r="AE48" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="76">
@@ -5530,1256 +6787,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AE48"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AD47" sqref="AD47:AE47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
-        <v>43061</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6">
-        <v>43062</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6">
-        <v>43063</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6">
-        <v>43064</v>
-      </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6">
-        <v>43065</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6">
-        <v>43066</v>
-      </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6">
-        <v>43067</v>
-      </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6">
-        <v>43068</v>
-      </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6">
-        <v>43069</v>
-      </c>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6">
-        <v>43070</v>
-      </c>
-      <c r="U5" s="6"/>
-      <c r="V5" s="6">
-        <v>43071</v>
-      </c>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6">
-        <v>43072</v>
-      </c>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6">
-        <v>43073</v>
-      </c>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6">
-        <v>43074</v>
-      </c>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="6">
-        <v>43075</v>
-      </c>
-      <c r="AE5" s="6"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="7">
-        <f>SUM(C11:C45)</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7">
-        <f>SUM(E11:E45)</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
-        <f>SUM(G11:G45)</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7">
-        <f t="shared" ref="H6" si="0">SUM(I11:I45)</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
-        <f>SUM(K11:K45)</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7">
-        <f t="shared" ref="L6" si="1">SUM(M11:M45)</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7">
-        <f t="shared" ref="N6" si="2">SUM(O11:O45)</f>
-        <v>0</v>
-      </c>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7">
-        <f>SUM(Q11:Q45)</f>
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7">
-        <f t="shared" ref="R6" si="3">SUM(S11:S45)</f>
-        <v>0</v>
-      </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7">
-        <f t="shared" ref="T6" si="4">SUM(U11:U45)</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7">
-        <f t="shared" ref="V6" si="5">SUM(W11:W45)</f>
-        <v>0</v>
-      </c>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7">
-        <f t="shared" ref="X6" si="6">SUM(Y11:Y45)</f>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7">
-        <f t="shared" ref="Z6" si="7">SUM(AA11:AA45)</f>
-        <v>0</v>
-      </c>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7">
-        <f t="shared" ref="AB6" si="8">SUM(AC11:AC45)</f>
-        <v>0</v>
-      </c>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7">
-        <f t="shared" ref="AD6" si="9">SUM(AE11:AE45)</f>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="7"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <f>B3-(SUM(B6:AD6))</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Z10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AD11" s="3"/>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Z12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AD12" s="3"/>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Z13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AD13" s="3"/>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Z14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AD14" s="3"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AD15" s="3"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AD16" s="3"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="R17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AD17" s="3"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="R18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AD18" s="3"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AD19" s="3"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Z20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AD20" s="3"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="L21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="X21" s="3"/>
-      <c r="Z21" s="3"/>
-      <c r="AB21" s="3"/>
-      <c r="AD21" s="3"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="L22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="V22" s="3"/>
-      <c r="X22" s="3"/>
-      <c r="Z22" s="3"/>
-      <c r="AB22" s="3"/>
-      <c r="AD22" s="3"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="V23" s="3"/>
-      <c r="X23" s="3"/>
-      <c r="Z23" s="3"/>
-      <c r="AB23" s="3"/>
-      <c r="AD23" s="3"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="R24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="V24" s="3"/>
-      <c r="X24" s="3"/>
-      <c r="Z24" s="3"/>
-      <c r="AB24" s="3"/>
-      <c r="AD24" s="3"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="N25" s="3"/>
-      <c r="P25" s="3"/>
-      <c r="R25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="V25" s="3"/>
-      <c r="X25" s="3"/>
-      <c r="Z25" s="3"/>
-      <c r="AB25" s="3"/>
-      <c r="AD25" s="3"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="R26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="V26" s="3"/>
-      <c r="X26" s="3"/>
-      <c r="Z26" s="3"/>
-      <c r="AB26" s="3"/>
-      <c r="AD26" s="3"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="L27" s="3"/>
-      <c r="N27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="X27" s="3"/>
-      <c r="Z27" s="3"/>
-      <c r="AB27" s="3"/>
-      <c r="AD27" s="3"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="N28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="R28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="X28" s="3"/>
-      <c r="Z28" s="3"/>
-      <c r="AB28" s="3"/>
-      <c r="AD28" s="3"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="L29" s="3"/>
-      <c r="N29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="X29" s="3"/>
-      <c r="Z29" s="3"/>
-      <c r="AB29" s="3"/>
-      <c r="AD29" s="3"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A30" s="4"/>
-      <c r="B30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Z30" s="3"/>
-      <c r="AB30" s="3"/>
-      <c r="AD30" s="3"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="X31" s="3"/>
-      <c r="Z31" s="3"/>
-      <c r="AB31" s="3"/>
-      <c r="AD31" s="3"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="R32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="X32" s="3"/>
-      <c r="Z32" s="3"/>
-      <c r="AB32" s="3"/>
-      <c r="AD32" s="3"/>
-    </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="V33" s="3"/>
-      <c r="X33" s="3"/>
-      <c r="Z33" s="3"/>
-      <c r="AB33" s="3"/>
-      <c r="AD33" s="3"/>
-    </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A34" s="4"/>
-      <c r="B34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="N34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="R34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="V34" s="3"/>
-      <c r="X34" s="3"/>
-      <c r="Z34" s="3"/>
-      <c r="AB34" s="3"/>
-      <c r="AD34" s="3"/>
-    </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="N35" s="3"/>
-      <c r="P35" s="3"/>
-      <c r="R35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="X35" s="3"/>
-      <c r="Z35" s="3"/>
-      <c r="AB35" s="3"/>
-      <c r="AD35" s="3"/>
-    </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A36" s="4"/>
-      <c r="B36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="R36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="X36" s="3"/>
-      <c r="Z36" s="3"/>
-      <c r="AB36" s="3"/>
-      <c r="AD36" s="3"/>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="N37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="R37" s="3"/>
-      <c r="T37" s="3"/>
-      <c r="V37" s="3"/>
-      <c r="X37" s="3"/>
-      <c r="Z37" s="3"/>
-      <c r="AB37" s="3"/>
-      <c r="AD37" s="3"/>
-    </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="T38" s="3"/>
-      <c r="V38" s="3"/>
-      <c r="X38" s="3"/>
-      <c r="Z38" s="3"/>
-      <c r="AB38" s="3"/>
-      <c r="AD38" s="3"/>
-    </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A39" s="4"/>
-      <c r="B39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="R39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="X39" s="3"/>
-      <c r="Z39" s="3"/>
-      <c r="AB39" s="3"/>
-      <c r="AD39" s="3"/>
-    </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A40" s="4"/>
-      <c r="B40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="N40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="R40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="X40" s="3"/>
-      <c r="Z40" s="3"/>
-      <c r="AB40" s="3"/>
-      <c r="AD40" s="3"/>
-    </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A41" s="4"/>
-      <c r="B41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="R41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="V41" s="3"/>
-      <c r="X41" s="3"/>
-      <c r="Z41" s="3"/>
-      <c r="AB41" s="3"/>
-      <c r="AD41" s="3"/>
-    </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AB42" s="3"/>
-      <c r="AD42" s="3"/>
-    </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AB43" s="3"/>
-      <c r="AD43" s="3"/>
-    </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A44" s="4"/>
-      <c r="B44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Z44" s="3"/>
-      <c r="AB44" s="3"/>
-      <c r="AD44" s="3"/>
-    </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A45" s="4"/>
-      <c r="B45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Z45" s="3"/>
-      <c r="AB45" s="3"/>
-      <c r="AD45" s="3"/>
-    </row>
-    <row r="46" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="6">
-        <f>B5</f>
-        <v>43061</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6">
-        <f t="shared" ref="D46:AE46" si="10">D5</f>
-        <v>43062</v>
-      </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6">
-        <f t="shared" ref="F46:AE46" si="11">F5</f>
-        <v>43063</v>
-      </c>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6">
-        <f t="shared" ref="H46:AE46" si="12">H5</f>
-        <v>43064</v>
-      </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6">
-        <f t="shared" ref="J46:AE46" si="13">J5</f>
-        <v>43065</v>
-      </c>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6">
-        <f t="shared" ref="L46:AE46" si="14">L5</f>
-        <v>43066</v>
-      </c>
-      <c r="M46" s="6"/>
-      <c r="N46" s="6">
-        <f t="shared" ref="N46:AE46" si="15">N5</f>
-        <v>43067</v>
-      </c>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6">
-        <f t="shared" ref="P46:AE46" si="16">P5</f>
-        <v>43068</v>
-      </c>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6">
-        <f t="shared" ref="R46:AE46" si="17">R5</f>
-        <v>43069</v>
-      </c>
-      <c r="S46" s="6"/>
-      <c r="T46" s="6">
-        <f t="shared" ref="T46:AE46" si="18">T5</f>
-        <v>43070</v>
-      </c>
-      <c r="U46" s="6"/>
-      <c r="V46" s="6">
-        <f t="shared" ref="V46:AE46" si="19">V5</f>
-        <v>43071</v>
-      </c>
-      <c r="W46" s="6"/>
-      <c r="X46" s="6">
-        <f t="shared" ref="X46:AE46" si="20">X5</f>
-        <v>43072</v>
-      </c>
-      <c r="Y46" s="6"/>
-      <c r="Z46" s="6">
-        <f t="shared" ref="Z46:AE46" si="21">Z5</f>
-        <v>43073</v>
-      </c>
-      <c r="AA46" s="6"/>
-      <c r="AB46" s="6">
-        <f t="shared" ref="AB46:AE46" si="22">AB5</f>
-        <v>43074</v>
-      </c>
-      <c r="AC46" s="6"/>
-      <c r="AD46" s="6">
-        <f>AD5</f>
-        <v>43075</v>
-      </c>
-      <c r="AE46" s="6"/>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="5">
-        <f>$B$3-B6</f>
-        <v>25</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5">
-        <f>B47-D6</f>
-        <v>25</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5">
-        <f>D47-F6</f>
-        <v>25</v>
-      </c>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5">
-        <f>F47-H6</f>
-        <v>25</v>
-      </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5">
-        <f>H47-J6</f>
-        <v>25</v>
-      </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5">
-        <f>J47-L6</f>
-        <v>25</v>
-      </c>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5">
-        <f>L47-N6</f>
-        <v>25</v>
-      </c>
-      <c r="O47" s="5"/>
-      <c r="P47" s="5">
-        <f>N47-P6</f>
-        <v>25</v>
-      </c>
-      <c r="Q47" s="5"/>
-      <c r="R47" s="5">
-        <f>P47-R6</f>
-        <v>25</v>
-      </c>
-      <c r="S47" s="5"/>
-      <c r="T47" s="5">
-        <f>R47-T6</f>
-        <v>25</v>
-      </c>
-      <c r="U47" s="5"/>
-      <c r="V47" s="5">
-        <f>T47-V6</f>
-        <v>25</v>
-      </c>
-      <c r="W47" s="5"/>
-      <c r="X47" s="5">
-        <f>V47-X6</f>
-        <v>25</v>
-      </c>
-      <c r="Y47" s="5"/>
-      <c r="Z47" s="5">
-        <f>X47-Z6</f>
-        <v>25</v>
-      </c>
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="5">
-        <f>Z47-AB6</f>
-        <v>25</v>
-      </c>
-      <c r="AC47" s="5"/>
-      <c r="AD47" s="5">
-        <f>AB47-AD6</f>
-        <v>25</v>
-      </c>
-      <c r="AE47" s="5"/>
-    </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="5">
-        <f>B3</f>
-        <v>25</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5">
-        <f>B48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>23.33</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5">
-        <f t="shared" ref="F48" si="23">D48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>21.659999999999997</v>
-      </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5">
-        <f t="shared" ref="H48" si="24">F48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>19.989999999999995</v>
-      </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5">
-        <f t="shared" ref="J48" si="25">H48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>18.319999999999993</v>
-      </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5">
-        <f t="shared" ref="L48" si="26">J48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>16.649999999999991</v>
-      </c>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5">
-        <f t="shared" ref="N48" si="27">L48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>14.979999999999992</v>
-      </c>
-      <c r="O48" s="5"/>
-      <c r="P48" s="5">
-        <f t="shared" ref="P48" si="28">N48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>13.309999999999992</v>
-      </c>
-      <c r="Q48" s="5"/>
-      <c r="R48" s="5">
-        <f t="shared" ref="R48" si="29">P48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>11.639999999999992</v>
-      </c>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5">
-        <f t="shared" ref="T48" si="30">R48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>9.9699999999999918</v>
-      </c>
-      <c r="U48" s="5"/>
-      <c r="V48" s="5">
-        <f t="shared" ref="V48" si="31">T48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>8.2999999999999918</v>
-      </c>
-      <c r="W48" s="5"/>
-      <c r="X48" s="5">
-        <f t="shared" ref="X48" si="32">V48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>6.6299999999999919</v>
-      </c>
-      <c r="Y48" s="5"/>
-      <c r="Z48" s="5">
-        <f t="shared" ref="Z48" si="33">X48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>4.959999999999992</v>
-      </c>
-      <c r="AA48" s="5"/>
-      <c r="AB48" s="5">
-        <f t="shared" ref="AB48" si="34">Z48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>3.289999999999992</v>
-      </c>
-      <c r="AC48" s="5"/>
-      <c r="AD48" s="5">
-        <f t="shared" ref="AD48" si="35">AB48-(ROUND(($B$3/COUNTA($B$46:$AD$46)*1),2))</f>
-        <v>1.6199999999999921</v>
-      </c>
-      <c r="AE48" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
-    <mergeCell ref="Z46:AA46"/>
-    <mergeCell ref="AB6:AC6"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="A10:A45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="T6:U6"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="X6:Y6"/>
-    <mergeCell ref="AB47:AC47"/>
-    <mergeCell ref="AB46:AC46"/>
-    <mergeCell ref="AD46:AE46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="P47:Q47"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="R46:S46"/>
-    <mergeCell ref="T46:U46"/>
-    <mergeCell ref="V46:W46"/>
-    <mergeCell ref="X46:Y46"/>
-    <mergeCell ref="AD48:AE48"/>
-    <mergeCell ref="AD47:AE47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="R48:S48"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="T47:U47"/>
-    <mergeCell ref="V47:W47"/>
-    <mergeCell ref="X47:Y47"/>
-    <mergeCell ref="Z47:AA47"/>
-    <mergeCell ref="T48:U48"/>
-    <mergeCell ref="V48:W48"/>
-    <mergeCell ref="X48:Y48"/>
-    <mergeCell ref="Z48:AA48"/>
-    <mergeCell ref="AB48:AC48"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>